<commit_message>
updating scripts for new JH data model; using different GDP effects calcuation on coronavirus costs
</commit_message>
<xml_diff>
--- a/Projects/COVID-19/Economic costs of coronavirus.xlsx
+++ b/Projects/COVID-19/Economic costs of coronavirus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csq\Documents\Public_Policy\Projects\COVID-19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAB440A-C93A-4623-8089-C18BAC77C731}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357B87C4-06E2-49EB-9050-54D2F90F2E3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2084352B-F601-49F1-8B25-E9FF30E33CA6}"/>
   </bookViews>
@@ -17,6 +17,41 @@
     <sheet name="Sources" sheetId="3" r:id="rId2"/>
     <sheet name="Screencaps" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Worksheet!$D$4</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Worksheet!$L$4</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Worksheet!$L$4</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Worksheet!$D$21</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
   <si>
     <t>https://www.bloomberg.com/graphics/2017-value-of-life/</t>
   </si>
@@ -315,6 +350,27 @@
   </si>
   <si>
     <t>Proportion critical, died</t>
+  </si>
+  <si>
+    <t>Worst Case Economic Situation vs. Current Policy</t>
+  </si>
+  <si>
+    <t>5 Year Annual Avg. Growth</t>
+  </si>
+  <si>
+    <t>Worst Case Loss</t>
+  </si>
+  <si>
+    <t>Typical Recession Growth</t>
+  </si>
+  <si>
+    <t>COVID-19 Impacts</t>
+  </si>
+  <si>
+    <t>Growth that would have occurred without COVID-19</t>
+  </si>
+  <si>
+    <t>Loss from Pre-COVID</t>
   </si>
 </sst>
 </file>
@@ -374,15 +430,21 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -645,6 +707,19 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -658,7 +733,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -710,9 +785,6 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -727,9 +799,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -747,24 +816,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -783,24 +834,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -808,15 +841,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -831,33 +855,6 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -867,13 +864,119 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1451,7 +1554,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B586A5-4885-4C36-A714-94AFC14C8180}">
-  <dimension ref="B2:Q44"/>
+  <dimension ref="B2:R44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
@@ -1464,12 +1567,12 @@
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:18" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
         <v>44</v>
       </c>
@@ -1483,28 +1586,46 @@
         <v>33</v>
       </c>
       <c r="F3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="L3" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="M3" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="97" t="s">
-        <v>93</v>
-      </c>
-      <c r="J3" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="K3" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="L3" s="44" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N3" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="O3" s="89" t="s">
+        <v>95</v>
+      </c>
+      <c r="P3" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q3" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="R3" s="43" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="15">
         <v>78.69</v>
       </c>
@@ -1519,40 +1640,61 @@
         <f>D4/80</f>
         <v>131088.77299999999</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="17">
+        <v>9763</v>
+      </c>
+      <c r="G4" s="17">
+        <v>20292</v>
+      </c>
+      <c r="H4" s="72">
+        <v>2.3E-2</v>
+      </c>
+      <c r="I4" s="44">
+        <f>0.05-H4</f>
+        <v>2.7000000000000003E-2</v>
+      </c>
+      <c r="J4" s="45">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K4" s="46">
+        <f>SUM(H4:J4)</f>
+        <v>0.19</v>
+      </c>
+      <c r="L4" s="77">
+        <v>0.5</v>
+      </c>
+      <c r="M4" s="19">
         <v>-3.7999999999999999E-2</v>
       </c>
-      <c r="G4" s="17">
-        <v>9763</v>
-      </c>
-      <c r="H4" s="17">
-        <v>20292</v>
-      </c>
-      <c r="I4" s="98">
+      <c r="N4" s="19">
+        <f>AVERAGE(O4,P4)</f>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="O4" s="90">
         <v>2.3E-2</v>
       </c>
-      <c r="J4" s="45">
-        <f>0.05-I4</f>
-        <v>2.7000000000000003E-2</v>
-      </c>
-      <c r="K4" s="46">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="L4" s="47">
-        <f>SUM(I4:K4)</f>
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P4" s="19">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Q4" s="44">
+        <f>(N4-M4)*-1</f>
+        <v>-5.0999999999999997E-2</v>
+      </c>
+      <c r="R4" s="91">
+        <f>Q4*L4</f>
+        <v>-2.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
       <c r="D5" s="30"/>
       <c r="E5" s="29"/>
       <c r="F5" s="23"/>
-      <c r="G5" s="42"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="30"/>
     </row>
-    <row r="6" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>75</v>
       </c>
@@ -1560,66 +1702,66 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="L6" s="95" t="s">
+      <c r="L6" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="95"/>
-      <c r="N6" s="95"/>
-      <c r="O6" s="95"/>
-      <c r="P6" s="95"/>
-    </row>
-    <row r="7" spans="2:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="89" t="s">
+      <c r="M6" s="78"/>
+      <c r="N6" s="78"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+    </row>
+    <row r="7" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="87" t="s">
+      <c r="C7" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="87" t="s">
+      <c r="D7" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="87" t="s">
+      <c r="E7" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="87" t="s">
+      <c r="F7" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="87" t="s">
+      <c r="G7" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="87" t="s">
+      <c r="H7" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="87" t="s">
+      <c r="I7" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="J7" s="87" t="s">
+      <c r="J7" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="87" t="s">
+      <c r="K7" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="93" t="s">
+      <c r="L7" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="M7" s="94"/>
-      <c r="N7" s="94"/>
-      <c r="O7" s="91" t="s">
+      <c r="M7" s="88"/>
+      <c r="N7" s="88"/>
+      <c r="O7" s="85" t="s">
         <v>83</v>
       </c>
-      <c r="P7" s="92"/>
-    </row>
-    <row r="8" spans="2:16" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="90"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="88"/>
-      <c r="I8" s="88"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
+      <c r="P7" s="86"/>
+    </row>
+    <row r="8" spans="2:18" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="81"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
       <c r="L8" s="12">
         <v>200000</v>
       </c>
@@ -1630,14 +1772,14 @@
       <c r="N8" s="13">
         <v>480000</v>
       </c>
-      <c r="O8" s="55">
+      <c r="O8" s="53">
         <v>1700000</v>
       </c>
       <c r="P8" s="14">
         <v>2200000</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="21" t="s">
         <v>2</v>
       </c>
@@ -1674,11 +1816,11 @@
         <f t="shared" ref="K9:K16" si="3">J9*$E$4</f>
         <v>274630.97943499981</v>
       </c>
-      <c r="L9" s="50">
+      <c r="L9" s="48">
         <f>L$8*$K9*$I9</f>
         <v>18086257868.122261</v>
       </c>
-      <c r="M9" s="53">
+      <c r="M9" s="51">
         <f t="shared" ref="M9:P16" si="4">M$8*$K9*$I9</f>
         <v>30746638375.807842</v>
       </c>
@@ -1686,7 +1828,7 @@
         <f t="shared" si="4"/>
         <v>43407018883.493423</v>
       </c>
-      <c r="O9" s="49">
+      <c r="O9" s="47">
         <f t="shared" si="4"/>
         <v>153733191879.03922</v>
       </c>
@@ -1695,7 +1837,7 @@
         <v>198948836549.34488</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="21" t="s">
         <v>3</v>
       </c>
@@ -1732,7 +1874,7 @@
         <f t="shared" si="3"/>
         <v>549261.95886999962</v>
       </c>
-      <c r="L10" s="50">
+      <c r="L10" s="48">
         <f t="shared" ref="L10:L16" si="7">L$8*$K10*$I10</f>
         <v>36326979931.069199</v>
       </c>
@@ -1744,7 +1886,7 @@
         <f t="shared" si="4"/>
         <v>87184751834.566071</v>
       </c>
-      <c r="O10" s="49">
+      <c r="O10" s="47">
         <f t="shared" si="4"/>
         <v>308779329414.0882</v>
       </c>
@@ -1753,7 +1895,7 @@
         <v>399596779241.76123</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="21" t="s">
         <v>7</v>
       </c>
@@ -1790,7 +1932,7 @@
         <f t="shared" si="3"/>
         <v>1860149.6888699995</v>
       </c>
-      <c r="L11" s="50">
+      <c r="L11" s="48">
         <f t="shared" si="7"/>
         <v>87751403699.309433</v>
       </c>
@@ -1802,7 +1944,7 @@
         <f t="shared" si="4"/>
         <v>210603368878.34265</v>
       </c>
-      <c r="O11" s="49">
+      <c r="O11" s="47">
         <f t="shared" si="4"/>
         <v>745886931444.13025</v>
       </c>
@@ -1811,7 +1953,7 @@
         <v>965265440692.40393</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="21" t="s">
         <v>8</v>
       </c>
@@ -1849,7 +1991,7 @@
         <f t="shared" si="3"/>
         <v>3171037.4188699992</v>
       </c>
-      <c r="L12" s="50">
+      <c r="L12" s="48">
         <f t="shared" si="7"/>
         <v>45902829393.875542</v>
       </c>
@@ -1861,7 +2003,7 @@
         <f t="shared" si="4"/>
         <v>110166790545.3013</v>
       </c>
-      <c r="O12" s="49">
+      <c r="O12" s="47">
         <f t="shared" si="4"/>
         <v>390174049847.94208</v>
       </c>
@@ -1870,7 +2012,7 @@
         <v>504931123332.63092</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="21" t="s">
         <v>9</v>
       </c>
@@ -1908,7 +2050,7 @@
         <f t="shared" si="3"/>
         <v>4481925.1488699997</v>
       </c>
-      <c r="L13" s="50">
+      <c r="L13" s="48">
         <f t="shared" si="7"/>
         <v>15519038285.214933</v>
       </c>
@@ -1920,7 +2062,7 @@
         <f t="shared" si="4"/>
         <v>37245691884.515846</v>
       </c>
-      <c r="O13" s="49">
+      <c r="O13" s="47">
         <f t="shared" si="4"/>
         <v>131911825424.32693</v>
       </c>
@@ -1929,7 +2071,7 @@
         <v>170709421137.36429</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="21" t="s">
         <v>10</v>
       </c>
@@ -1967,7 +2109,7 @@
         <f t="shared" si="3"/>
         <v>5792812.8788699992</v>
       </c>
-      <c r="L14" s="50">
+      <c r="L14" s="48">
         <f t="shared" si="7"/>
         <v>11469755442.986298</v>
       </c>
@@ -1979,7 +2121,7 @@
         <f t="shared" si="4"/>
         <v>27527413063.167114</v>
       </c>
-      <c r="O14" s="49">
+      <c r="O14" s="47">
         <f t="shared" si="4"/>
         <v>97492921265.38353</v>
       </c>
@@ -1988,7 +2130,7 @@
         <v>126167309872.84927</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" s="21" t="s">
         <v>11</v>
       </c>
@@ -2026,7 +2168,7 @@
         <f t="shared" si="3"/>
         <v>7103700.6088699987</v>
       </c>
-      <c r="L15" s="50">
+      <c r="L15" s="48">
         <f t="shared" si="7"/>
         <v>5449123651.0538206</v>
       </c>
@@ -2038,7 +2180,7 @@
         <f t="shared" si="4"/>
         <v>13077896762.529171</v>
       </c>
-      <c r="O15" s="49">
+      <c r="O15" s="47">
         <f t="shared" si="4"/>
         <v>46317551033.957474</v>
       </c>
@@ -2047,7 +2189,7 @@
         <v>59940360161.592033</v>
       </c>
     </row>
-    <row r="16" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="33" t="s">
         <v>12</v>
       </c>
@@ -2085,7 +2227,7 @@
         <f t="shared" si="3"/>
         <v>8414588.3388699982</v>
       </c>
-      <c r="L16" s="51">
+      <c r="L16" s="49">
         <f t="shared" si="7"/>
         <v>1227871100.2333059</v>
       </c>
@@ -2097,7 +2239,7 @@
         <f t="shared" si="4"/>
         <v>2946890640.5599341</v>
       </c>
-      <c r="O16" s="52">
+      <c r="O16" s="50">
         <f t="shared" si="4"/>
         <v>10436904351.983099</v>
       </c>
@@ -2107,7 +2249,7 @@
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B17" s="41"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="22"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -2124,7 +2266,7 @@
       <c r="P17" s="30"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B18" s="41"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="22"/>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
@@ -2141,7 +2283,7 @@
       <c r="P18" s="30"/>
     </row>
     <row r="19" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="41"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="22"/>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
@@ -2150,12 +2292,14 @@
       <c r="H19" s="26"/>
       <c r="I19" s="27"/>
       <c r="J19" s="28"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="95"/>
-      <c r="M19" s="95"/>
-      <c r="N19" s="95"/>
-      <c r="O19" s="95"/>
-      <c r="P19" s="95"/>
+      <c r="K19" s="92" t="s">
+        <v>98</v>
+      </c>
+      <c r="L19" s="78"/>
+      <c r="M19" s="78"/>
+      <c r="N19" s="78"/>
+      <c r="O19" s="78"/>
+      <c r="P19" s="78"/>
     </row>
     <row r="20" spans="2:17" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D20" s="2"/>
@@ -2163,39 +2307,40 @@
       <c r="F20" s="2"/>
       <c r="H20" s="4"/>
       <c r="I20" s="5"/>
-      <c r="K20" s="102"/>
-      <c r="L20" s="90" t="s">
+      <c r="K20" s="74"/>
+      <c r="L20" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="M20" s="88"/>
-      <c r="N20" s="88"/>
-      <c r="O20" s="100" t="s">
+      <c r="M20" s="80"/>
+      <c r="N20" s="80"/>
+      <c r="O20" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="P20" s="101"/>
+      <c r="P20" s="83"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D21" s="2"/>
       <c r="H21" s="4"/>
-      <c r="K21" s="39" t="s">
+      <c r="K21" s="93" t="s">
         <v>90</v>
       </c>
-      <c r="L21" s="58">
+      <c r="L21" s="102">
         <f>L8</f>
         <v>200000</v>
       </c>
-      <c r="M21" s="59">
+      <c r="M21" s="103">
         <f t="shared" ref="M21:P21" si="8">M8</f>
         <v>340000</v>
       </c>
-      <c r="N21" s="59">
+      <c r="N21" s="103">
         <f t="shared" si="8"/>
         <v>480000</v>
       </c>
-      <c r="O21" s="58">
+      <c r="O21" s="102">
         <f t="shared" si="8"/>
         <v>1700000</v>
       </c>
-      <c r="P21" s="60">
+      <c r="P21" s="104">
         <f t="shared" si="8"/>
         <v>2200000</v>
       </c>
@@ -2204,251 +2349,251 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="H22" s="4"/>
-      <c r="K22" s="40" t="s">
+      <c r="K22" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="L22" s="84">
-        <f>L21*($J$4/$I$4)</f>
+      <c r="L22" s="67">
+        <f>L21*($I$4/$H$4)</f>
         <v>234782.60869565219</v>
       </c>
-      <c r="M22" s="85">
-        <f t="shared" ref="M22:P22" si="9">M21*($J$4/$I$4)</f>
+      <c r="M22" s="68">
+        <f t="shared" ref="M22:P22" si="9">M21*($I$4/$H$4)</f>
         <v>399130.4347826087</v>
       </c>
-      <c r="N22" s="85">
+      <c r="N22" s="68">
         <f t="shared" si="9"/>
         <v>563478.2608695653</v>
       </c>
-      <c r="O22" s="84">
+      <c r="O22" s="67">
         <f t="shared" si="9"/>
         <v>1995652.1739130437</v>
       </c>
-      <c r="P22" s="86">
+      <c r="P22" s="69">
         <f t="shared" si="9"/>
         <v>2582608.6956521743</v>
       </c>
-      <c r="Q22" s="96"/>
+      <c r="Q22" s="70"/>
     </row>
     <row r="23" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="H23" s="4"/>
-      <c r="K23" s="48" t="s">
+      <c r="K23" s="105" t="s">
         <v>92</v>
       </c>
-      <c r="L23" s="61">
-        <f>SUM(L21,L22)*($K$4/($I$4+$J$4))</f>
+      <c r="L23" s="106">
+        <f>SUM(L21,L22)*($J$4/($H$4+$I$4))</f>
         <v>1217391.3043478264</v>
       </c>
-      <c r="M23" s="62">
-        <f t="shared" ref="M23:P23" si="10">SUM(M21,M22)*($K$4/($I$4+$J$4))</f>
+      <c r="M23" s="107">
+        <f t="shared" ref="M23:P23" si="10">SUM(M21,M22)*($J$4/($H$4+$I$4))</f>
         <v>2069565.2173913044</v>
       </c>
-      <c r="N23" s="62">
+      <c r="N23" s="107">
         <f t="shared" si="10"/>
         <v>2921739.1304347832</v>
       </c>
-      <c r="O23" s="61">
+      <c r="O23" s="106">
         <f t="shared" si="10"/>
         <v>10347826.086956523</v>
       </c>
-      <c r="P23" s="63">
+      <c r="P23" s="108">
         <f t="shared" si="10"/>
         <v>13391304.347826088</v>
       </c>
     </row>
     <row r="24" spans="2:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H24" s="4"/>
-      <c r="K24" s="57" t="s">
+      <c r="K24" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="L24" s="76">
+      <c r="L24" s="62">
         <f>SUM(L8,L21,L23)</f>
         <v>1617391.3043478264</v>
       </c>
-      <c r="M24" s="77">
+      <c r="M24" s="63">
         <f>SUM(M8,M21,M23)</f>
         <v>2749565.2173913047</v>
       </c>
-      <c r="N24" s="77">
+      <c r="N24" s="63">
         <f>SUM(N8,N21,N23)</f>
         <v>3881739.1304347832</v>
       </c>
-      <c r="O24" s="76">
+      <c r="O24" s="62">
         <f>SUM(O8,O21,O23)</f>
         <v>13747826.086956523</v>
       </c>
-      <c r="P24" s="78">
+      <c r="P24" s="64">
         <f>SUM(P8,P21,P23)</f>
         <v>17791304.347826086</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="H25" s="4"/>
-      <c r="K25" s="82"/>
-      <c r="L25" s="99"/>
-      <c r="M25" s="99"/>
-      <c r="N25" s="99"/>
-      <c r="O25" s="99"/>
-      <c r="P25" s="99"/>
+      <c r="K25" s="65"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="73"/>
+      <c r="N25" s="73"/>
+      <c r="O25" s="73"/>
+      <c r="P25" s="73"/>
     </row>
     <row r="26" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H26" s="4"/>
-      <c r="K26" s="83" t="s">
+      <c r="K26" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="L26" s="77"/>
-      <c r="M26" s="77"/>
-      <c r="N26" s="77"/>
-      <c r="O26" s="77"/>
-      <c r="P26" s="77"/>
+      <c r="L26" s="63"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="63"/>
+      <c r="O26" s="63"/>
+      <c r="P26" s="63"/>
     </row>
     <row r="27" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="K27" s="39" t="s">
+      <c r="K27" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="L27" s="79">
+      <c r="L27" s="94">
         <f>SUM(L9:L16)</f>
         <v>221733259371.86481</v>
       </c>
-      <c r="M27" s="80">
+      <c r="M27" s="95">
         <f>SUM(M9:M16)</f>
         <v>376946540932.1701</v>
       </c>
-      <c r="N27" s="80">
+      <c r="N27" s="95">
         <f>SUM(N9:N16)</f>
         <v>532159822492.47559</v>
       </c>
-      <c r="O27" s="79">
+      <c r="O27" s="94">
         <f>SUM(O9:O16)</f>
         <v>1884732704660.8511</v>
       </c>
-      <c r="P27" s="81">
+      <c r="P27" s="96">
         <f>SUM(P9:P16)</f>
         <v>2439065853090.5127</v>
       </c>
     </row>
     <row r="28" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="K28" s="40" t="s">
+      <c r="K28" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="L28" s="64">
-        <f>L23*$G$4</f>
+      <c r="L28" s="56">
+        <f>L23*$F$4</f>
         <v>11885391304.34783</v>
       </c>
-      <c r="M28" s="65">
-        <f t="shared" ref="M28:P28" si="11">M23*$G$4</f>
+      <c r="M28" s="57">
+        <f t="shared" ref="M28:P28" si="11">M23*$F$4</f>
         <v>20205165217.391304</v>
       </c>
-      <c r="N28" s="65">
+      <c r="N28" s="57">
         <f t="shared" si="11"/>
         <v>28524939130.434788</v>
       </c>
-      <c r="O28" s="64">
+      <c r="O28" s="56">
         <f t="shared" si="11"/>
         <v>101025826086.95654</v>
       </c>
-      <c r="P28" s="66">
+      <c r="P28" s="58">
         <f t="shared" si="11"/>
         <v>130739304347.8261</v>
       </c>
     </row>
     <row r="29" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="K29" s="40" t="s">
+      <c r="K29" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="L29" s="64">
-        <f>SUM(L21,L22)*$H$4</f>
+      <c r="L29" s="98">
+        <f>SUM(L21,L22)*$G$4</f>
         <v>8822608695.652174</v>
       </c>
-      <c r="M29" s="65">
-        <f t="shared" ref="M29:P29" si="12">SUM(M21,M22)*$H$4</f>
+      <c r="M29" s="99">
+        <f t="shared" ref="M29:P29" si="12">SUM(M21,M22)*$G$4</f>
         <v>14998434782.608694</v>
       </c>
-      <c r="N29" s="65">
+      <c r="N29" s="99">
         <f t="shared" si="12"/>
         <v>21174260869.56522</v>
       </c>
-      <c r="O29" s="64">
+      <c r="O29" s="98">
         <f t="shared" si="12"/>
         <v>74992173913.043488</v>
       </c>
-      <c r="P29" s="66">
+      <c r="P29" s="100">
         <f t="shared" si="12"/>
         <v>97048695652.173904</v>
       </c>
     </row>
     <row r="30" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="K30" s="56" t="s">
+      <c r="K30" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="L30" s="67">
+      <c r="L30" s="59">
         <f>SUM(L27:L29)</f>
         <v>242441259371.86481</v>
       </c>
-      <c r="M30" s="68">
+      <c r="M30" s="60">
         <f>SUM(M27:M29)</f>
         <v>412150140932.1701</v>
       </c>
-      <c r="N30" s="68">
+      <c r="N30" s="60">
         <f>SUM(N27:N29)</f>
         <v>581859022492.47559</v>
       </c>
-      <c r="O30" s="67">
+      <c r="O30" s="59">
         <f>SUM(O27:O29)</f>
         <v>2060750704660.8511</v>
       </c>
-      <c r="P30" s="69">
+      <c r="P30" s="61">
         <f>SUM(P27:P29)</f>
         <v>2666853853090.5127</v>
       </c>
     </row>
     <row r="31" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K31" s="57" t="s">
+      <c r="K31" s="101" t="s">
         <v>71</v>
       </c>
-      <c r="L31" s="70">
+      <c r="L31" s="109">
         <f>L30/$C$4*-1</f>
         <v>-1.1544821874850704E-2</v>
       </c>
-      <c r="M31" s="71">
+      <c r="M31" s="110">
         <f t="shared" ref="M31:P31" si="13">M30/$C$4*-1</f>
         <v>-1.9626197187246196E-2</v>
       </c>
-      <c r="N31" s="71">
+      <c r="N31" s="110">
         <f t="shared" si="13"/>
         <v>-2.7707572499641696E-2</v>
       </c>
-      <c r="O31" s="70">
+      <c r="O31" s="109">
         <f t="shared" si="13"/>
         <v>-9.8130985936230999E-2</v>
       </c>
-      <c r="P31" s="72">
+      <c r="P31" s="111">
         <f t="shared" si="13"/>
         <v>-0.12699304062335776</v>
       </c>
     </row>
     <row r="32" spans="2:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K32" s="54" t="s">
+      <c r="K32" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="L32" s="73">
-        <f>L31+$F$4</f>
-        <v>-4.9544821874850702E-2</v>
-      </c>
-      <c r="M32" s="74">
-        <f>M31+$F$4</f>
-        <v>-5.7626197187246195E-2</v>
-      </c>
-      <c r="N32" s="74">
-        <f>N31+$F$4</f>
-        <v>-6.5707572499641695E-2</v>
-      </c>
-      <c r="O32" s="73">
-        <f>O31+0.5*$F$4</f>
-        <v>-0.117130985936231</v>
-      </c>
-      <c r="P32" s="75">
-        <f>P31+0.5*$F$4</f>
-        <v>-0.14599304062335774</v>
+      <c r="L32" s="112">
+        <f>L31+$Q$4</f>
+        <v>-6.2544821874850706E-2</v>
+      </c>
+      <c r="M32" s="113">
+        <f t="shared" ref="M32:N32" si="14">M31+$Q$4</f>
+        <v>-7.0626197187246192E-2</v>
+      </c>
+      <c r="N32" s="113">
+        <f t="shared" si="14"/>
+        <v>-7.8707572499641693E-2</v>
+      </c>
+      <c r="O32" s="112">
+        <f>O31+$R$4</f>
+        <v>-0.12363098593623099</v>
+      </c>
+      <c r="P32" s="114">
+        <f>P31+$R$4</f>
+        <v>-0.15249304062335775</v>
       </c>
     </row>
     <row r="33" spans="11:16" x14ac:dyDescent="0.3">
@@ -2458,6 +2603,9 @@
     </row>
     <row r="34" spans="11:16" x14ac:dyDescent="0.3">
       <c r="O34" s="2"/>
+    </row>
+    <row r="35" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="P35" s="5"/>
     </row>
     <row r="37" spans="11:16" x14ac:dyDescent="0.3">
       <c r="K37" s="2"/>
@@ -2514,12 +2662,12 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="O7:P7"/>
     <mergeCell ref="L7:N7"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="L6:P6"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="D7:D8"/>
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="I7:I8"/>

</xml_diff>

<commit_message>
working on some finance scripts, saving older stuff
</commit_message>
<xml_diff>
--- a/Projects/COVID-19/Economic costs of coronavirus.xlsx
+++ b/Projects/COVID-19/Economic costs of coronavirus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csq\Documents\Public_Policy\Projects\COVID-19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D7D6BE-F373-4CC8-8FBE-E97088A07825}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A88D77-6D63-49B2-A290-DCE3B786899D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{2084352B-F601-49F1-8B25-E9FF30E33CA6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2084352B-F601-49F1-8B25-E9FF30E33CA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -68,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="106">
   <si>
     <t>https://www.bloomberg.com/graphics/2017-value-of-life/</t>
   </si>
@@ -208,9 +210,6 @@
     <t>Economic Forecast, Goldman Sachs</t>
   </si>
   <si>
-    <t>2020 Economic Forecast, Goldman Sachs</t>
-  </si>
-  <si>
     <t>Coronavirus Statistics</t>
   </si>
   <si>
@@ -371,6 +370,24 @@
   </si>
   <si>
     <t>Loss from Pre-COVID</t>
+  </si>
+  <si>
+    <t>Value of Statistical Life-Year</t>
+  </si>
+  <si>
+    <t>https://papers.ssrn.com/sol3/papers.cfm?abstract_id=3379967</t>
+  </si>
+  <si>
+    <t>IMF October Projection</t>
+  </si>
+  <si>
+    <t>3 Year Average Growth</t>
+  </si>
+  <si>
+    <t>2020 Economic Forecast, Goldman Sachs, March</t>
+  </si>
+  <si>
+    <t>Deaths at Median Mortality</t>
   </si>
 </sst>
 </file>
@@ -444,7 +461,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -723,6 +740,30 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -733,7 +774,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -944,24 +985,27 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -977,6 +1021,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1554,25 +1610,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B586A5-4885-4C36-A714-94AFC14C8180}">
-  <dimension ref="B2:R44"/>
+  <dimension ref="B2:T44"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="10" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" customWidth="1"/>
-    <col min="12" max="15" width="21.44140625" customWidth="1"/>
-    <col min="16" max="16" width="24.5546875" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" customWidth="1"/>
+    <col min="12" max="16" width="21.42578125" customWidth="1"/>
+    <col min="17" max="17" width="24.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>44</v>
       </c>
@@ -1586,46 +1646,52 @@
         <v>33</v>
       </c>
       <c r="F3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>50</v>
-      </c>
       <c r="H3" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="I3" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="K3" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="L3" s="76" t="s">
+      <c r="M3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="N3" s="104" t="s">
+        <v>102</v>
+      </c>
+      <c r="O3" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="P3" s="78" t="s">
         <v>94</v>
       </c>
-      <c r="M3" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="N3" s="75" t="s">
+      <c r="Q3" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="R3" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="S3" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="O3" s="78" t="s">
+      <c r="T3" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="P3" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q3" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="R3" s="43" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="15">
         <v>78.69</v>
       </c>
@@ -1667,25 +1733,31 @@
         <v>-3.7999999999999999E-2</v>
       </c>
       <c r="N4" s="19">
-        <f>AVERAGE(O4,P4)</f>
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="O4" s="79">
+        <v>-4.2999999999999997E-2</v>
+      </c>
+      <c r="O4" s="19">
+        <f>Q4</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="P4" s="79">
         <v>2.3E-2</v>
       </c>
-      <c r="P4" s="19">
+      <c r="Q4" s="19">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="R4" s="19">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="Q4" s="44">
-        <f>(N4-M4)*-1</f>
-        <v>-5.0999999999999997E-2</v>
-      </c>
-      <c r="R4" s="80">
-        <f>Q4*L4</f>
-        <v>-2.5499999999999998E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="S4" s="44">
+        <f>1-(1+O4)/(1+N4)</f>
+        <v>-7.1055381400208839E-2</v>
+      </c>
+      <c r="T4" s="80">
+        <f>S4*L4</f>
+        <v>-3.552769070010442E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
       <c r="D5" s="30"/>
@@ -1694,92 +1766,99 @@
       <c r="G5" s="41"/>
       <c r="H5" s="30"/>
     </row>
-    <row r="6" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="L6" s="104" t="s">
+      <c r="L6" s="105" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="104"/>
-      <c r="N6" s="104"/>
-      <c r="O6" s="104"/>
-      <c r="P6" s="104"/>
-    </row>
-    <row r="7" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="110" t="s">
+      <c r="M6" s="105"/>
+      <c r="N6" s="105"/>
+      <c r="O6" s="105"/>
+      <c r="P6" s="105"/>
+      <c r="Q6" s="105"/>
+    </row>
+    <row r="7" spans="2:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="109" t="s">
+      <c r="C7" s="106" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="109" t="s">
+      <c r="D7" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="109" t="s">
+      <c r="E7" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="109" t="s">
+      <c r="F7" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="109" t="s">
+      <c r="G7" s="106" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="109" t="s">
+      <c r="H7" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="109" t="s">
-        <v>81</v>
-      </c>
-      <c r="J7" s="109" t="s">
+      <c r="I7" s="106" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="109" t="s">
+      <c r="K7" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="113" t="s">
-        <v>84</v>
-      </c>
-      <c r="M7" s="114"/>
-      <c r="N7" s="114"/>
-      <c r="O7" s="111" t="s">
+      <c r="L7" s="117" t="s">
+        <v>105</v>
+      </c>
+      <c r="M7" s="114" t="s">
         <v>83</v>
       </c>
-      <c r="P7" s="112"/>
-    </row>
-    <row r="8" spans="2:18" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="105"/>
-      <c r="C8" s="106"/>
-      <c r="D8" s="106"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="106"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="106"/>
-      <c r="I8" s="106"/>
-      <c r="J8" s="106"/>
-      <c r="K8" s="106"/>
-      <c r="L8" s="12">
+      <c r="N7" s="115"/>
+      <c r="O7" s="116"/>
+      <c r="P7" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q7" s="113"/>
+    </row>
+    <row r="8" spans="2:20" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="108"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="107"/>
+      <c r="G8" s="107"/>
+      <c r="H8" s="107"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="107"/>
+      <c r="K8" s="107"/>
+      <c r="L8" s="118">
+        <v>60000</v>
+      </c>
+      <c r="M8" s="12">
         <v>200000</v>
       </c>
-      <c r="M8" s="13">
-        <f>AVERAGE(L8,N8)</f>
+      <c r="N8" s="13">
+        <f>AVERAGE(M8,O8)</f>
         <v>340000</v>
       </c>
-      <c r="N8" s="13">
+      <c r="O8" s="13">
         <v>480000</v>
       </c>
-      <c r="O8" s="53">
+      <c r="P8" s="53">
         <v>1700000</v>
       </c>
-      <c r="P8" s="14">
+      <c r="Q8" s="14">
         <v>2200000</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
         <v>2</v>
       </c>
@@ -1816,28 +1895,32 @@
         <f t="shared" ref="K9:K16" si="3">J9*$E$4</f>
         <v>274630.97943499981</v>
       </c>
-      <c r="L9" s="48">
-        <f>L$8*$K9*$I9</f>
+      <c r="L9" s="119">
+        <f t="shared" ref="L9:L16" si="4">L$8*$K9*$I9</f>
+        <v>5425877360.4366779</v>
+      </c>
+      <c r="M9" s="48">
+        <f>M$8*$K9*$I9</f>
         <v>18086257868.122261</v>
       </c>
-      <c r="M9" s="51">
-        <f t="shared" ref="M9:P16" si="4">M$8*$K9*$I9</f>
+      <c r="N9" s="51">
+        <f t="shared" ref="N9:Q16" si="5">N$8*$K9*$I9</f>
         <v>30746638375.807842</v>
       </c>
-      <c r="N9" s="30">
-        <f t="shared" si="4"/>
+      <c r="O9" s="30">
+        <f t="shared" si="5"/>
         <v>43407018883.493423</v>
       </c>
-      <c r="O9" s="47">
-        <f t="shared" si="4"/>
+      <c r="P9" s="47">
+        <f t="shared" si="5"/>
         <v>153733191879.03922</v>
       </c>
-      <c r="P9" s="31">
-        <f t="shared" si="4"/>
+      <c r="Q9" s="31">
+        <f t="shared" si="5"/>
         <v>198948836549.34488</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
         <v>3</v>
       </c>
@@ -1863,39 +1946,43 @@
         <v>2.3182390377541454E-2</v>
       </c>
       <c r="I10" s="27">
-        <f t="shared" ref="I10:I16" si="5">$H10/SUM($H$9:$H$16)</f>
+        <f t="shared" ref="I10:I16" si="6">$H10/SUM($H$9:$H$16)</f>
         <v>0.33068902137155959</v>
       </c>
       <c r="J10" s="28">
-        <f t="shared" ref="J10:J16" si="6">$B$4-C10</f>
+        <f t="shared" ref="J10:J16" si="7">$B$4-C10</f>
         <v>4.1899999999999977</v>
       </c>
       <c r="K10" s="29">
         <f t="shared" si="3"/>
         <v>549261.95886999962</v>
       </c>
-      <c r="L10" s="48">
-        <f t="shared" ref="L10:L16" si="7">L$8*$K10*$I10</f>
+      <c r="L10" s="119">
+        <f t="shared" si="4"/>
+        <v>10898093979.320759</v>
+      </c>
+      <c r="M10" s="48">
+        <f t="shared" ref="M10:M16" si="8">M$8*$K10*$I10</f>
         <v>36326979931.069199</v>
       </c>
-      <c r="M10" s="30">
-        <f t="shared" si="4"/>
+      <c r="N10" s="30">
+        <f t="shared" si="5"/>
         <v>61755865882.817635</v>
       </c>
-      <c r="N10" s="30">
-        <f t="shared" si="4"/>
+      <c r="O10" s="30">
+        <f t="shared" si="5"/>
         <v>87184751834.566071</v>
       </c>
-      <c r="O10" s="47">
-        <f t="shared" si="4"/>
+      <c r="P10" s="47">
+        <f t="shared" si="5"/>
         <v>308779329414.0882</v>
       </c>
-      <c r="P10" s="31">
-        <f t="shared" si="4"/>
+      <c r="Q10" s="31">
+        <f t="shared" si="5"/>
         <v>399596779241.76123</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
         <v>7</v>
       </c>
@@ -1921,39 +2008,43 @@
         <v>1.6535396780933971E-2</v>
       </c>
       <c r="I11" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.23587188768828737</v>
       </c>
       <c r="J11" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14.189999999999998</v>
       </c>
       <c r="K11" s="29">
         <f t="shared" si="3"/>
         <v>1860149.6888699995</v>
       </c>
-      <c r="L11" s="48">
-        <f t="shared" si="7"/>
+      <c r="L11" s="119">
+        <f t="shared" si="4"/>
+        <v>26325421109.792831</v>
+      </c>
+      <c r="M11" s="48">
+        <f t="shared" si="8"/>
         <v>87751403699.309433</v>
       </c>
-      <c r="M11" s="30">
-        <f t="shared" si="4"/>
+      <c r="N11" s="30">
+        <f t="shared" si="5"/>
         <v>149177386288.82605</v>
       </c>
-      <c r="N11" s="30">
-        <f t="shared" si="4"/>
+      <c r="O11" s="30">
+        <f t="shared" si="5"/>
         <v>210603368878.34265</v>
       </c>
-      <c r="O11" s="47">
-        <f t="shared" si="4"/>
+      <c r="P11" s="47">
+        <f t="shared" si="5"/>
         <v>745886931444.13025</v>
       </c>
-      <c r="P11" s="31">
-        <f t="shared" si="4"/>
+      <c r="Q11" s="31">
+        <f t="shared" si="5"/>
         <v>965265440692.40393</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="21" t="s">
         <v>8</v>
       </c>
@@ -1980,39 +2071,43 @@
         <v>5.0739540647277903E-3</v>
       </c>
       <c r="I12" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.2378252493521561E-2</v>
       </c>
       <c r="J12" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24.189999999999998</v>
       </c>
       <c r="K12" s="29">
         <f t="shared" si="3"/>
         <v>3171037.4188699992</v>
       </c>
-      <c r="L12" s="48">
-        <f t="shared" si="7"/>
+      <c r="L12" s="119">
+        <f t="shared" si="4"/>
+        <v>13770848818.162663</v>
+      </c>
+      <c r="M12" s="48">
+        <f t="shared" si="8"/>
         <v>45902829393.875542</v>
       </c>
-      <c r="M12" s="30">
-        <f t="shared" si="4"/>
+      <c r="N12" s="30">
+        <f t="shared" si="5"/>
         <v>78034809969.588409</v>
       </c>
-      <c r="N12" s="30">
-        <f t="shared" si="4"/>
+      <c r="O12" s="30">
+        <f t="shared" si="5"/>
         <v>110166790545.3013</v>
       </c>
-      <c r="O12" s="47">
-        <f t="shared" si="4"/>
+      <c r="P12" s="47">
+        <f t="shared" si="5"/>
         <v>390174049847.94208</v>
       </c>
-      <c r="P12" s="31">
-        <f t="shared" si="4"/>
+      <c r="Q12" s="31">
+        <f t="shared" si="5"/>
         <v>504931123332.63092</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
         <v>9</v>
       </c>
@@ -2039,39 +2134,43 @@
         <v>1.2136924421305186E-3</v>
       </c>
       <c r="I13" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.7312915510344539E-2</v>
       </c>
       <c r="J13" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>34.19</v>
       </c>
       <c r="K13" s="29">
         <f t="shared" si="3"/>
         <v>4481925.1488699997</v>
       </c>
-      <c r="L13" s="48">
-        <f t="shared" si="7"/>
+      <c r="L13" s="119">
+        <f t="shared" si="4"/>
+        <v>4655711485.5644808</v>
+      </c>
+      <c r="M13" s="48">
+        <f t="shared" si="8"/>
         <v>15519038285.214933</v>
       </c>
-      <c r="M13" s="30">
-        <f t="shared" si="4"/>
+      <c r="N13" s="30">
+        <f t="shared" si="5"/>
         <v>26382365084.865387</v>
       </c>
-      <c r="N13" s="30">
-        <f t="shared" si="4"/>
+      <c r="O13" s="30">
+        <f t="shared" si="5"/>
         <v>37245691884.515846</v>
       </c>
-      <c r="O13" s="47">
-        <f t="shared" si="4"/>
+      <c r="P13" s="47">
+        <f t="shared" si="5"/>
         <v>131911825424.32693</v>
       </c>
-      <c r="P13" s="31">
-        <f t="shared" si="4"/>
+      <c r="Q13" s="31">
+        <f t="shared" si="5"/>
         <v>170709421137.36429</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
         <v>10</v>
       </c>
@@ -2098,39 +2197,43 @@
         <v>6.9402178066598982E-4</v>
       </c>
       <c r="I14" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.8999878667094948E-3</v>
       </c>
       <c r="J14" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44.19</v>
       </c>
       <c r="K14" s="29">
         <f t="shared" si="3"/>
         <v>5792812.8788699992</v>
       </c>
-      <c r="L14" s="48">
-        <f t="shared" si="7"/>
+      <c r="L14" s="119">
+        <f t="shared" si="4"/>
+        <v>3440926632.8958893</v>
+      </c>
+      <c r="M14" s="48">
+        <f t="shared" si="8"/>
         <v>11469755442.986298</v>
       </c>
-      <c r="M14" s="30">
-        <f t="shared" si="4"/>
+      <c r="N14" s="30">
+        <f t="shared" si="5"/>
         <v>19498584253.076706</v>
       </c>
-      <c r="N14" s="30">
-        <f t="shared" si="4"/>
+      <c r="O14" s="30">
+        <f t="shared" si="5"/>
         <v>27527413063.167114</v>
       </c>
-      <c r="O14" s="47">
-        <f t="shared" si="4"/>
+      <c r="P14" s="47">
+        <f t="shared" si="5"/>
         <v>97492921265.38353</v>
       </c>
-      <c r="P14" s="31">
-        <f t="shared" si="4"/>
+      <c r="Q14" s="31">
+        <f t="shared" si="5"/>
         <v>126167309872.84927</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
         <v>11</v>
       </c>
@@ -2157,39 +2260,43 @@
         <v>2.6887502004314625E-4</v>
       </c>
       <c r="I15" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.8354119571493489E-3</v>
       </c>
       <c r="J15" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>54.19</v>
       </c>
       <c r="K15" s="29">
         <f t="shared" si="3"/>
         <v>7103700.6088699987</v>
       </c>
-      <c r="L15" s="48">
-        <f t="shared" si="7"/>
+      <c r="L15" s="119">
+        <f t="shared" si="4"/>
+        <v>1634737095.3161464</v>
+      </c>
+      <c r="M15" s="48">
+        <f t="shared" si="8"/>
         <v>5449123651.0538206</v>
       </c>
-      <c r="M15" s="30">
-        <f t="shared" si="4"/>
+      <c r="N15" s="30">
+        <f t="shared" si="5"/>
         <v>9263510206.7914963</v>
       </c>
-      <c r="N15" s="30">
-        <f t="shared" si="4"/>
+      <c r="O15" s="30">
+        <f t="shared" si="5"/>
         <v>13077896762.529171</v>
       </c>
-      <c r="O15" s="47">
-        <f t="shared" si="4"/>
+      <c r="P15" s="47">
+        <f t="shared" si="5"/>
         <v>46317551033.957474</v>
       </c>
-      <c r="P15" s="31">
-        <f t="shared" si="4"/>
+      <c r="Q15" s="31">
+        <f t="shared" si="5"/>
         <v>59940360161.592033</v>
       </c>
     </row>
-    <row r="16" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="33" t="s">
         <v>12</v>
       </c>
@@ -2216,39 +2323,43 @@
         <v>5.1147963410911205E-5</v>
       </c>
       <c r="I16" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.296085386383843E-4</v>
       </c>
       <c r="J16" s="38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>64.19</v>
       </c>
       <c r="K16" s="18">
         <f t="shared" si="3"/>
         <v>8414588.3388699982</v>
       </c>
-      <c r="L16" s="49">
-        <f t="shared" si="7"/>
+      <c r="L16" s="120">
+        <f t="shared" si="4"/>
+        <v>368361330.06999177</v>
+      </c>
+      <c r="M16" s="49">
+        <f t="shared" si="8"/>
         <v>1227871100.2333059</v>
       </c>
-      <c r="M16" s="17">
-        <f t="shared" si="4"/>
+      <c r="N16" s="17">
+        <f t="shared" si="5"/>
         <v>2087380870.3966198</v>
       </c>
-      <c r="N16" s="17">
-        <f t="shared" si="4"/>
+      <c r="O16" s="17">
+        <f t="shared" si="5"/>
         <v>2946890640.5599341</v>
       </c>
-      <c r="O16" s="50">
-        <f t="shared" si="4"/>
+      <c r="P16" s="50">
+        <f t="shared" si="5"/>
         <v>10436904351.983099</v>
       </c>
-      <c r="P16" s="20">
-        <f t="shared" si="4"/>
+      <c r="Q16" s="20">
+        <f t="shared" si="5"/>
         <v>13506582102.566364</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="40"/>
       <c r="C17" s="22"/>
       <c r="D17" s="23"/>
@@ -2264,8 +2375,9 @@
       <c r="N17" s="30"/>
       <c r="O17" s="30"/>
       <c r="P17" s="30"/>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q17" s="30"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="40"/>
       <c r="C18" s="22"/>
       <c r="D18" s="23"/>
@@ -2281,8 +2393,9 @@
       <c r="N18" s="30"/>
       <c r="O18" s="30"/>
       <c r="P18" s="30"/>
-    </row>
-    <row r="19" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q18" s="30"/>
+    </row>
+    <row r="19" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="40"/>
       <c r="C19" s="22"/>
       <c r="D19" s="23"/>
@@ -2293,140 +2406,160 @@
       <c r="I19" s="27"/>
       <c r="J19" s="28"/>
       <c r="K19" s="81" t="s">
-        <v>98</v>
-      </c>
-      <c r="L19" s="104"/>
-      <c r="M19" s="104"/>
-      <c r="N19" s="104"/>
-      <c r="O19" s="104"/>
-      <c r="P19" s="104"/>
-    </row>
-    <row r="20" spans="2:17" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="L19" s="121"/>
+      <c r="M19" s="121"/>
+      <c r="N19" s="121"/>
+      <c r="O19" s="121"/>
+      <c r="P19" s="121"/>
+      <c r="Q19" s="121"/>
+    </row>
+    <row r="20" spans="2:18" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="H20" s="4"/>
       <c r="I20" s="5"/>
       <c r="K20" s="74"/>
-      <c r="L20" s="105" t="s">
-        <v>84</v>
-      </c>
-      <c r="M20" s="106"/>
-      <c r="N20" s="106"/>
-      <c r="O20" s="107" t="s">
+      <c r="L20" s="117" t="s">
+        <v>105</v>
+      </c>
+      <c r="M20" s="114" t="s">
         <v>83</v>
       </c>
-      <c r="P20" s="108"/>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N20" s="115"/>
+      <c r="O20" s="116"/>
+      <c r="P20" s="109" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q20" s="110"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D21" s="2"/>
       <c r="H21" s="4"/>
       <c r="K21" s="82" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L21" s="91">
         <f>L8</f>
+        <v>60000</v>
+      </c>
+      <c r="M21" s="91">
+        <f>M8</f>
         <v>200000</v>
       </c>
-      <c r="M21" s="92">
-        <f t="shared" ref="M21:P21" si="8">M8</f>
+      <c r="N21" s="92">
+        <f t="shared" ref="N21:Q21" si="9">N8</f>
         <v>340000</v>
       </c>
-      <c r="N21" s="92">
-        <f t="shared" si="8"/>
+      <c r="O21" s="92">
+        <f t="shared" si="9"/>
         <v>480000</v>
       </c>
-      <c r="O21" s="91">
-        <f t="shared" si="8"/>
+      <c r="P21" s="91">
+        <f t="shared" si="9"/>
         <v>1700000</v>
       </c>
-      <c r="P21" s="93">
-        <f t="shared" si="8"/>
+      <c r="Q21" s="93">
+        <f t="shared" si="9"/>
         <v>2200000</v>
       </c>
     </row>
-    <row r="22" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="H22" s="4"/>
       <c r="K22" s="39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L22" s="67">
         <f>L21*($I$4/$H$4)</f>
+        <v>70434.782608695663</v>
+      </c>
+      <c r="M22" s="67">
+        <f>M21*($I$4/$H$4)</f>
         <v>234782.60869565219</v>
       </c>
-      <c r="M22" s="68">
-        <f t="shared" ref="M22:P22" si="9">M21*($I$4/$H$4)</f>
+      <c r="N22" s="68">
+        <f t="shared" ref="N22:Q22" si="10">N21*($I$4/$H$4)</f>
         <v>399130.4347826087</v>
       </c>
-      <c r="N22" s="68">
-        <f t="shared" si="9"/>
+      <c r="O22" s="68">
+        <f t="shared" si="10"/>
         <v>563478.2608695653</v>
       </c>
-      <c r="O22" s="67">
-        <f t="shared" si="9"/>
+      <c r="P22" s="67">
+        <f t="shared" si="10"/>
         <v>1995652.1739130437</v>
       </c>
-      <c r="P22" s="69">
-        <f t="shared" si="9"/>
+      <c r="Q22" s="69">
+        <f t="shared" si="10"/>
         <v>2582608.6956521743</v>
       </c>
-      <c r="Q22" s="70"/>
-    </row>
-    <row r="23" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="R22" s="70"/>
+    </row>
+    <row r="23" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="H23" s="4"/>
       <c r="K23" s="94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L23" s="95">
         <f>SUM(L21,L22)*($J$4/($H$4+$I$4))</f>
+        <v>365217.3913043479</v>
+      </c>
+      <c r="M23" s="95">
+        <f>SUM(M21,M22)*($J$4/($H$4+$I$4))</f>
         <v>1217391.3043478264</v>
       </c>
-      <c r="M23" s="96">
-        <f t="shared" ref="M23:P23" si="10">SUM(M21,M22)*($J$4/($H$4+$I$4))</f>
+      <c r="N23" s="96">
+        <f t="shared" ref="N23:Q23" si="11">SUM(N21,N22)*($J$4/($H$4+$I$4))</f>
         <v>2069565.2173913044</v>
       </c>
-      <c r="N23" s="96">
-        <f t="shared" si="10"/>
+      <c r="O23" s="96">
+        <f t="shared" si="11"/>
         <v>2921739.1304347832</v>
       </c>
-      <c r="O23" s="95">
-        <f t="shared" si="10"/>
+      <c r="P23" s="95">
+        <f t="shared" si="11"/>
         <v>10347826.086956523</v>
       </c>
-      <c r="P23" s="97">
-        <f t="shared" si="10"/>
+      <c r="Q23" s="97">
+        <f t="shared" si="11"/>
         <v>13391304.347826088</v>
       </c>
     </row>
-    <row r="24" spans="2:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H24" s="4"/>
       <c r="K24" s="55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L24" s="62">
         <f>SUM(L8,L21,L23)</f>
+        <v>485217.3913043479</v>
+      </c>
+      <c r="M24" s="62">
+        <f>SUM(M8,M21,M23)</f>
         <v>1617391.3043478264</v>
-      </c>
-      <c r="M24" s="63">
-        <f>SUM(M8,M21,M23)</f>
-        <v>2749565.2173913047</v>
       </c>
       <c r="N24" s="63">
         <f>SUM(N8,N21,N23)</f>
+        <v>2749565.2173913047</v>
+      </c>
+      <c r="O24" s="63">
+        <f>SUM(O8,O21,O23)</f>
         <v>3881739.1304347832</v>
       </c>
-      <c r="O24" s="62">
-        <f>SUM(O8,O21,O23)</f>
+      <c r="P24" s="62">
+        <f>SUM(P8,P21,P23)</f>
         <v>13747826.086956523</v>
       </c>
-      <c r="P24" s="64">
-        <f>SUM(P8,P21,P23)</f>
+      <c r="Q24" s="64">
+        <f>SUM(Q8,Q21,Q23)</f>
         <v>17791304.347826086</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H25" s="4"/>
       <c r="K25" s="65"/>
       <c r="L25" s="73"/>
@@ -2434,228 +2567,269 @@
       <c r="N25" s="73"/>
       <c r="O25" s="73"/>
       <c r="P25" s="73"/>
-    </row>
-    <row r="26" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q25" s="73"/>
+    </row>
+    <row r="26" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H26" s="4"/>
       <c r="K26" s="66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L26" s="63"/>
       <c r="M26" s="63"/>
       <c r="N26" s="63"/>
       <c r="O26" s="63"/>
       <c r="P26" s="63"/>
-    </row>
-    <row r="27" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q26" s="63"/>
+    </row>
+    <row r="27" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="K27" s="82" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L27" s="83">
         <f>SUM(L9:L16)</f>
+        <v>66519977811.559448</v>
+      </c>
+      <c r="M27" s="83">
+        <f>SUM(M9:M16)</f>
         <v>221733259371.86481</v>
-      </c>
-      <c r="M27" s="84">
-        <f>SUM(M9:M16)</f>
-        <v>376946540932.1701</v>
       </c>
       <c r="N27" s="84">
         <f>SUM(N9:N16)</f>
+        <v>376946540932.1701</v>
+      </c>
+      <c r="O27" s="84">
+        <f>SUM(O9:O16)</f>
         <v>532159822492.47559</v>
       </c>
-      <c r="O27" s="83">
-        <f>SUM(O9:O16)</f>
+      <c r="P27" s="83">
+        <f>SUM(P9:P16)</f>
         <v>1884732704660.8511</v>
       </c>
-      <c r="P27" s="85">
-        <f>SUM(P9:P16)</f>
+      <c r="Q27" s="85">
+        <f>SUM(Q9:Q16)</f>
         <v>2439065853090.5127</v>
       </c>
     </row>
-    <row r="28" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="K28" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L28" s="56">
         <f>L23*$F$4</f>
+        <v>3565617391.3043485</v>
+      </c>
+      <c r="M28" s="56">
+        <f>M23*$F$4</f>
         <v>11885391304.34783</v>
       </c>
-      <c r="M28" s="57">
-        <f t="shared" ref="M28:P28" si="11">M23*$F$4</f>
+      <c r="N28" s="57">
+        <f t="shared" ref="N28:Q28" si="12">N23*$F$4</f>
         <v>20205165217.391304</v>
       </c>
-      <c r="N28" s="57">
-        <f t="shared" si="11"/>
+      <c r="O28" s="57">
+        <f t="shared" si="12"/>
         <v>28524939130.434788</v>
       </c>
-      <c r="O28" s="56">
-        <f t="shared" si="11"/>
+      <c r="P28" s="56">
+        <f t="shared" si="12"/>
         <v>101025826086.95654</v>
       </c>
-      <c r="P28" s="58">
-        <f t="shared" si="11"/>
+      <c r="Q28" s="58">
+        <f t="shared" si="12"/>
         <v>130739304347.8261</v>
       </c>
     </row>
-    <row r="29" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="K29" s="86" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L29" s="87">
         <f>SUM(L21,L22)*$G$4</f>
+        <v>2646782608.6956525</v>
+      </c>
+      <c r="M29" s="87">
+        <f>SUM(M21,M22)*$G$4</f>
         <v>8822608695.652174</v>
       </c>
-      <c r="M29" s="88">
-        <f t="shared" ref="M29:P29" si="12">SUM(M21,M22)*$G$4</f>
+      <c r="N29" s="88">
+        <f t="shared" ref="N29:Q29" si="13">SUM(N21,N22)*$G$4</f>
         <v>14998434782.608694</v>
       </c>
-      <c r="N29" s="88">
-        <f t="shared" si="12"/>
+      <c r="O29" s="88">
+        <f t="shared" si="13"/>
         <v>21174260869.56522</v>
       </c>
-      <c r="O29" s="87">
-        <f t="shared" si="12"/>
+      <c r="P29" s="87">
+        <f t="shared" si="13"/>
         <v>74992173913.043488</v>
       </c>
-      <c r="P29" s="89">
-        <f t="shared" si="12"/>
+      <c r="Q29" s="89">
+        <f t="shared" si="13"/>
         <v>97048695652.173904</v>
       </c>
     </row>
-    <row r="30" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="K30" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L30" s="59">
         <f>SUM(L27:L29)</f>
+        <v>72732377811.559448</v>
+      </c>
+      <c r="M30" s="59">
+        <f>SUM(M27:M29)</f>
         <v>242441259371.86481</v>
-      </c>
-      <c r="M30" s="60">
-        <f>SUM(M27:M29)</f>
-        <v>412150140932.1701</v>
       </c>
       <c r="N30" s="60">
         <f>SUM(N27:N29)</f>
+        <v>412150140932.1701</v>
+      </c>
+      <c r="O30" s="60">
+        <f>SUM(O27:O29)</f>
         <v>581859022492.47559</v>
       </c>
-      <c r="O30" s="59">
-        <f>SUM(O27:O29)</f>
+      <c r="P30" s="59">
+        <f>SUM(P27:P29)</f>
         <v>2060750704660.8511</v>
       </c>
-      <c r="P30" s="61">
-        <f>SUM(P27:P29)</f>
+      <c r="Q30" s="61">
+        <f>SUM(Q27:Q29)</f>
         <v>2666853853090.5127</v>
       </c>
     </row>
-    <row r="31" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K31" s="90" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L31" s="98">
         <f>L30/$C$4*-1</f>
+        <v>-3.463446562455212E-3</v>
+      </c>
+      <c r="M31" s="98">
+        <f>M30/$C$4*-1</f>
         <v>-1.1544821874850704E-2</v>
       </c>
-      <c r="M31" s="99">
-        <f t="shared" ref="M31:P31" si="13">M30/$C$4*-1</f>
+      <c r="N31" s="99">
+        <f t="shared" ref="N31:Q31" si="14">N30/$C$4*-1</f>
         <v>-1.9626197187246196E-2</v>
       </c>
-      <c r="N31" s="99">
-        <f t="shared" si="13"/>
+      <c r="O31" s="99">
+        <f t="shared" si="14"/>
         <v>-2.7707572499641696E-2</v>
       </c>
-      <c r="O31" s="98">
-        <f t="shared" si="13"/>
+      <c r="P31" s="98">
+        <f t="shared" si="14"/>
         <v>-9.8130985936230999E-2</v>
       </c>
-      <c r="P31" s="100">
-        <f t="shared" si="13"/>
+      <c r="Q31" s="100">
+        <f t="shared" si="14"/>
         <v>-0.12699304062335776</v>
       </c>
     </row>
-    <row r="32" spans="2:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:18" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K32" s="52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L32" s="101">
-        <f>L31+$Q$4</f>
-        <v>-6.2544821874850706E-2</v>
-      </c>
-      <c r="M32" s="102">
-        <f t="shared" ref="M32:N32" si="14">M31+$Q$4</f>
-        <v>-7.0626197187246192E-2</v>
+        <f>L31+$S$4</f>
+        <v>-7.4518827962664055E-2</v>
+      </c>
+      <c r="M32" s="101">
+        <f>M31+$S$4</f>
+        <v>-8.2600203275059542E-2</v>
       </c>
       <c r="N32" s="102">
-        <f t="shared" si="14"/>
-        <v>-7.8707572499641693E-2</v>
-      </c>
-      <c r="O32" s="101">
-        <f>O31+$R$4</f>
-        <v>-0.12363098593623099</v>
-      </c>
-      <c r="P32" s="103">
-        <f>P31+$R$4</f>
-        <v>-0.15249304062335775</v>
-      </c>
-    </row>
-    <row r="33" spans="11:16" x14ac:dyDescent="0.3">
+        <f>N31+$S$4</f>
+        <v>-9.0681578587455042E-2</v>
+      </c>
+      <c r="O32" s="102">
+        <f>O31+$S$4</f>
+        <v>-9.8762953899850542E-2</v>
+      </c>
+      <c r="P32" s="101">
+        <f>P31+$T$4</f>
+        <v>-0.13365867663633541</v>
+      </c>
+      <c r="Q32" s="103">
+        <f>Q31+$T$4</f>
+        <v>-0.16252073132346218</v>
+      </c>
+    </row>
+    <row r="33" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="O34" s="2"/>
-    </row>
-    <row r="35" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="P35" s="5"/>
-    </row>
-    <row r="37" spans="11:16" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="P34" s="2"/>
+    </row>
+    <row r="35" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="Q35" s="5"/>
+    </row>
+    <row r="37" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K37" s="2"/>
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
-    </row>
-    <row r="38" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="Q37" s="6"/>
+    </row>
+    <row r="38" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K38" s="3"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
-    </row>
-    <row r="39" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="Q38" s="2"/>
+    </row>
+    <row r="39" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
-    </row>
-    <row r="40" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
-    </row>
-    <row r="41" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
-    </row>
-    <row r="42" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="N41" s="2"/>
+    </row>
+    <row r="42" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
-    </row>
-    <row r="43" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
-    </row>
-    <row r="44" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="N43" s="2"/>
+    </row>
+    <row r="44" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="L6:P6"/>
+  <mergeCells count="15">
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="L6:Q6"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="F7:F8"/>
@@ -2663,14 +2837,6 @@
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="L19:P19"/>
-    <mergeCell ref="L20:N20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2679,21 +2845,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7BF6D1-AC08-47EC-B644-0F220400F590}">
-  <dimension ref="A2:C25"/>
+  <dimension ref="A2:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="44.33203125" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
@@ -2701,18 +2867,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2723,7 +2889,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2734,7 +2900,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2745,7 +2911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2756,7 +2922,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2767,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2778,7 +2944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2789,7 +2955,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2800,7 +2966,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2811,7 +2977,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2822,7 +2988,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2830,128 +2996,139 @@
         <v>45</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>89</v>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2990,7 +3167,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
life lears lost plot
</commit_message>
<xml_diff>
--- a/Projects/COVID-19/Economic costs of coronavirus.xlsx
+++ b/Projects/COVID-19/Economic costs of coronavirus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csq\Documents\Public_Policy\Projects\COVID-19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csq\Documents\Public_Policy_Upd\Projects\COVID-19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A88D77-6D63-49B2-A290-DCE3B786899D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D617B975-DD70-4FBA-81DE-4B8A619AF9FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2084352B-F601-49F1-8B25-E9FF30E33CA6}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" xr2:uid="{2084352B-F601-49F1-8B25-E9FF30E33CA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -988,42 +988,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1033,6 +997,42 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1774,71 +1774,71 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="L6" s="105" t="s">
+      <c r="L6" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="105"/>
-      <c r="N6" s="105"/>
-      <c r="O6" s="105"/>
-      <c r="P6" s="105"/>
-      <c r="Q6" s="105"/>
+      <c r="M6" s="121"/>
+      <c r="N6" s="121"/>
+      <c r="O6" s="121"/>
+      <c r="P6" s="121"/>
+      <c r="Q6" s="121"/>
     </row>
     <row r="7" spans="2:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="111" t="s">
+      <c r="B7" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="106" t="s">
+      <c r="C7" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="106" t="s">
+      <c r="D7" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="106" t="s">
+      <c r="E7" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="106" t="s">
+      <c r="F7" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="106" t="s">
+      <c r="G7" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="106" t="s">
+      <c r="H7" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="106" t="s">
+      <c r="I7" s="112" t="s">
         <v>80</v>
       </c>
-      <c r="J7" s="106" t="s">
+      <c r="J7" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="106" t="s">
+      <c r="K7" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="117" t="s">
+      <c r="L7" s="105" t="s">
         <v>105</v>
       </c>
-      <c r="M7" s="114" t="s">
+      <c r="M7" s="118" t="s">
         <v>83</v>
       </c>
-      <c r="N7" s="115"/>
-      <c r="O7" s="116"/>
-      <c r="P7" s="112" t="s">
+      <c r="N7" s="119"/>
+      <c r="O7" s="120"/>
+      <c r="P7" s="116" t="s">
         <v>82</v>
       </c>
-      <c r="Q7" s="113"/>
+      <c r="Q7" s="117"/>
     </row>
     <row r="8" spans="2:20" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="108"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="107"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="107"/>
-      <c r="G8" s="107"/>
-      <c r="H8" s="107"/>
-      <c r="I8" s="107"/>
-      <c r="J8" s="107"/>
-      <c r="K8" s="107"/>
-      <c r="L8" s="118">
+      <c r="B8" s="115"/>
+      <c r="C8" s="113"/>
+      <c r="D8" s="113"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="113"/>
+      <c r="G8" s="113"/>
+      <c r="H8" s="113"/>
+      <c r="I8" s="113"/>
+      <c r="J8" s="113"/>
+      <c r="K8" s="113"/>
+      <c r="L8" s="106">
         <v>60000</v>
       </c>
       <c r="M8" s="12">
@@ -1895,7 +1895,7 @@
         <f t="shared" ref="K9:K16" si="3">J9*$E$4</f>
         <v>274630.97943499981</v>
       </c>
-      <c r="L9" s="119">
+      <c r="L9" s="107">
         <f t="shared" ref="L9:L16" si="4">L$8*$K9*$I9</f>
         <v>5425877360.4366779</v>
       </c>
@@ -1957,7 +1957,7 @@
         <f t="shared" si="3"/>
         <v>549261.95886999962</v>
       </c>
-      <c r="L10" s="119">
+      <c r="L10" s="107">
         <f t="shared" si="4"/>
         <v>10898093979.320759</v>
       </c>
@@ -2019,7 +2019,7 @@
         <f t="shared" si="3"/>
         <v>1860149.6888699995</v>
       </c>
-      <c r="L11" s="119">
+      <c r="L11" s="107">
         <f t="shared" si="4"/>
         <v>26325421109.792831</v>
       </c>
@@ -2082,7 +2082,7 @@
         <f t="shared" si="3"/>
         <v>3171037.4188699992</v>
       </c>
-      <c r="L12" s="119">
+      <c r="L12" s="107">
         <f t="shared" si="4"/>
         <v>13770848818.162663</v>
       </c>
@@ -2145,7 +2145,7 @@
         <f t="shared" si="3"/>
         <v>4481925.1488699997</v>
       </c>
-      <c r="L13" s="119">
+      <c r="L13" s="107">
         <f t="shared" si="4"/>
         <v>4655711485.5644808</v>
       </c>
@@ -2208,7 +2208,7 @@
         <f t="shared" si="3"/>
         <v>5792812.8788699992</v>
       </c>
-      <c r="L14" s="119">
+      <c r="L14" s="107">
         <f t="shared" si="4"/>
         <v>3440926632.8958893</v>
       </c>
@@ -2271,7 +2271,7 @@
         <f t="shared" si="3"/>
         <v>7103700.6088699987</v>
       </c>
-      <c r="L15" s="119">
+      <c r="L15" s="107">
         <f t="shared" si="4"/>
         <v>1634737095.3161464</v>
       </c>
@@ -2334,7 +2334,7 @@
         <f t="shared" si="3"/>
         <v>8414588.3388699982</v>
       </c>
-      <c r="L16" s="120">
+      <c r="L16" s="108">
         <f t="shared" si="4"/>
         <v>368361330.06999177</v>
       </c>
@@ -2408,12 +2408,12 @@
       <c r="K19" s="81" t="s">
         <v>97</v>
       </c>
-      <c r="L19" s="121"/>
-      <c r="M19" s="121"/>
-      <c r="N19" s="121"/>
-      <c r="O19" s="121"/>
-      <c r="P19" s="121"/>
-      <c r="Q19" s="121"/>
+      <c r="L19" s="109"/>
+      <c r="M19" s="109"/>
+      <c r="N19" s="109"/>
+      <c r="O19" s="109"/>
+      <c r="P19" s="109"/>
+      <c r="Q19" s="109"/>
     </row>
     <row r="20" spans="2:18" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="2"/>
@@ -2422,18 +2422,18 @@
       <c r="H20" s="4"/>
       <c r="I20" s="5"/>
       <c r="K20" s="74"/>
-      <c r="L20" s="117" t="s">
+      <c r="L20" s="105" t="s">
         <v>105</v>
       </c>
-      <c r="M20" s="114" t="s">
+      <c r="M20" s="118" t="s">
         <v>83</v>
       </c>
-      <c r="N20" s="115"/>
-      <c r="O20" s="116"/>
-      <c r="P20" s="109" t="s">
+      <c r="N20" s="119"/>
+      <c r="O20" s="120"/>
+      <c r="P20" s="110" t="s">
         <v>82</v>
       </c>
-      <c r="Q20" s="110"/>
+      <c r="Q20" s="111"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D21" s="2"/>
@@ -2535,27 +2535,27 @@
         <v>81</v>
       </c>
       <c r="L24" s="62">
-        <f>SUM(L8,L21,L23)</f>
+        <f t="shared" ref="L24:Q24" si="12">SUM(L8,L21,L23)</f>
         <v>485217.3913043479</v>
       </c>
       <c r="M24" s="62">
-        <f>SUM(M8,M21,M23)</f>
+        <f t="shared" si="12"/>
         <v>1617391.3043478264</v>
       </c>
       <c r="N24" s="63">
-        <f>SUM(N8,N21,N23)</f>
+        <f t="shared" si="12"/>
         <v>2749565.2173913047</v>
       </c>
       <c r="O24" s="63">
-        <f>SUM(O8,O21,O23)</f>
+        <f t="shared" si="12"/>
         <v>3881739.1304347832</v>
       </c>
       <c r="P24" s="62">
-        <f>SUM(P8,P21,P23)</f>
+        <f t="shared" si="12"/>
         <v>13747826.086956523</v>
       </c>
       <c r="Q24" s="64">
-        <f>SUM(Q8,Q21,Q23)</f>
+        <f t="shared" si="12"/>
         <v>17791304.347826086</v>
       </c>
     </row>
@@ -2586,27 +2586,27 @@
         <v>69</v>
       </c>
       <c r="L27" s="83">
-        <f>SUM(L9:L16)</f>
+        <f t="shared" ref="L27:Q27" si="13">SUM(L9:L16)</f>
         <v>66519977811.559448</v>
       </c>
       <c r="M27" s="83">
-        <f>SUM(M9:M16)</f>
+        <f t="shared" si="13"/>
         <v>221733259371.86481</v>
       </c>
       <c r="N27" s="84">
-        <f>SUM(N9:N16)</f>
+        <f t="shared" si="13"/>
         <v>376946540932.1701</v>
       </c>
       <c r="O27" s="84">
-        <f>SUM(O9:O16)</f>
+        <f t="shared" si="13"/>
         <v>532159822492.47559</v>
       </c>
       <c r="P27" s="83">
-        <f>SUM(P9:P16)</f>
+        <f t="shared" si="13"/>
         <v>1884732704660.8511</v>
       </c>
       <c r="Q27" s="85">
-        <f>SUM(Q9:Q16)</f>
+        <f t="shared" si="13"/>
         <v>2439065853090.5127</v>
       </c>
     </row>
@@ -2623,19 +2623,19 @@
         <v>11885391304.34783</v>
       </c>
       <c r="N28" s="57">
-        <f t="shared" ref="N28:Q28" si="12">N23*$F$4</f>
+        <f t="shared" ref="N28:Q28" si="14">N23*$F$4</f>
         <v>20205165217.391304</v>
       </c>
       <c r="O28" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>28524939130.434788</v>
       </c>
       <c r="P28" s="56">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>101025826086.95654</v>
       </c>
       <c r="Q28" s="58">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>130739304347.8261</v>
       </c>
     </row>
@@ -2652,19 +2652,19 @@
         <v>8822608695.652174</v>
       </c>
       <c r="N29" s="88">
-        <f t="shared" ref="N29:Q29" si="13">SUM(N21,N22)*$G$4</f>
+        <f t="shared" ref="N29:Q29" si="15">SUM(N21,N22)*$G$4</f>
         <v>14998434782.608694</v>
       </c>
       <c r="O29" s="88">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>21174260869.56522</v>
       </c>
       <c r="P29" s="87">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>74992173913.043488</v>
       </c>
       <c r="Q29" s="89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>97048695652.173904</v>
       </c>
     </row>
@@ -2673,27 +2673,27 @@
         <v>85</v>
       </c>
       <c r="L30" s="59">
-        <f>SUM(L27:L29)</f>
+        <f t="shared" ref="L30:Q30" si="16">SUM(L27:L29)</f>
         <v>72732377811.559448</v>
       </c>
       <c r="M30" s="59">
-        <f>SUM(M27:M29)</f>
+        <f t="shared" si="16"/>
         <v>242441259371.86481</v>
       </c>
       <c r="N30" s="60">
-        <f>SUM(N27:N29)</f>
+        <f t="shared" si="16"/>
         <v>412150140932.1701</v>
       </c>
       <c r="O30" s="60">
-        <f>SUM(O27:O29)</f>
+        <f t="shared" si="16"/>
         <v>581859022492.47559</v>
       </c>
       <c r="P30" s="59">
-        <f>SUM(P27:P29)</f>
+        <f t="shared" si="16"/>
         <v>2060750704660.8511</v>
       </c>
       <c r="Q30" s="61">
-        <f>SUM(Q27:Q29)</f>
+        <f t="shared" si="16"/>
         <v>2666853853090.5127</v>
       </c>
     </row>
@@ -2710,19 +2710,19 @@
         <v>-1.1544821874850704E-2</v>
       </c>
       <c r="N31" s="99">
-        <f t="shared" ref="N31:Q31" si="14">N30/$C$4*-1</f>
+        <f t="shared" ref="N31:Q31" si="17">N30/$C$4*-1</f>
         <v>-1.9626197187246196E-2</v>
       </c>
       <c r="O31" s="99">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-2.7707572499641696E-2</v>
       </c>
       <c r="P31" s="98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-9.8130985936230999E-2</v>
       </c>
       <c r="Q31" s="100">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-0.12699304062335776</v>
       </c>
     </row>
@@ -2822,13 +2822,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M20:O20"/>
     <mergeCell ref="L6:Q6"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="G7:G8"/>
@@ -2837,6 +2830,13 @@
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="I7:I8"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M20:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
some cleanup, new tab in economics workbook
</commit_message>
<xml_diff>
--- a/Projects/COVID-19/Economic costs of coronavirus.xlsx
+++ b/Projects/COVID-19/Economic costs of coronavirus.xlsx
@@ -8,48 +8,82 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csq\Documents\Public_Policy_Upd\Projects\COVID-19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D617B975-DD70-4FBA-81DE-4B8A619AF9FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDD1B1C-C91B-4973-AD68-2C86FEA9BE2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" xr2:uid="{2084352B-F601-49F1-8B25-E9FF30E33CA6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{2084352B-F601-49F1-8B25-E9FF30E33CA6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Sources" sheetId="3" r:id="rId2"/>
-    <sheet name="Screencaps" sheetId="4" r:id="rId3"/>
+    <sheet name="March 2020" sheetId="1" r:id="rId1"/>
+    <sheet name="January 2021" sheetId="5" r:id="rId2"/>
+    <sheet name="Sources" sheetId="3" r:id="rId3"/>
+    <sheet name="Screencaps" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Worksheet!$D$4</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'January 2021'!$C$4</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'March 2020'!$D$4</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Worksheet!$L$4</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Worksheet!$L$4</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'January 2021'!#REF!</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'March 2020'!$L$4</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'January 2021'!#REF!</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'March 2020'!$L$4</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Worksheet!$D$21</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'January 2021'!$D$24</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'March 2020'!$D$21</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -70,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="128">
   <si>
     <t>https://www.bloomberg.com/graphics/2017-value-of-life/</t>
   </si>
@@ -388,19 +422,86 @@
   </si>
   <si>
     <t>Deaths at Median Mortality</t>
+  </si>
+  <si>
+    <t>85+</t>
+  </si>
+  <si>
+    <t>75-84</t>
+  </si>
+  <si>
+    <t>65-74</t>
+  </si>
+  <si>
+    <t>55-64</t>
+  </si>
+  <si>
+    <t>45-54</t>
+  </si>
+  <si>
+    <t>35-44</t>
+  </si>
+  <si>
+    <t>25-34</t>
+  </si>
+  <si>
+    <t>15-24</t>
+  </si>
+  <si>
+    <t>5-14</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>&lt;1</t>
+  </si>
+  <si>
+    <t>Fatalities as of Dec 30, 2020</t>
+  </si>
+  <si>
+    <t>Mortality Rate per 100k</t>
+  </si>
+  <si>
+    <t>Counted Deaths (CDC)</t>
+  </si>
+  <si>
+    <t>Excess Deaths (CDC)</t>
+  </si>
+  <si>
+    <t>Counted Deaths (Johns Hopkins)</t>
+  </si>
+  <si>
+    <t>Fatality Share</t>
+  </si>
+  <si>
+    <t>Value of Life Lost by Age Group</t>
+  </si>
+  <si>
+    <t>Lost Growth Relative Pre-COVID Path</t>
+  </si>
+  <si>
+    <t>Cumulative Hospitalizations (COVID Tracking Project)</t>
+  </si>
+  <si>
+    <t>Cost of treatment</t>
+  </si>
+  <si>
+    <t>https://www.cnbc.com/2020/04/09/heres-what-you-need-to-know-about-coronavirus-treatment-costs.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="0.0000000000000000%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -461,7 +562,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -763,6 +864,69 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -774,7 +938,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -997,18 +1161,27 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1030,9 +1203,67 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="31" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1612,7 +1843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B586A5-4885-4C36-A714-94AFC14C8180}">
   <dimension ref="B2:T44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1736,8 +1967,8 @@
         <v>-4.2999999999999997E-2</v>
       </c>
       <c r="O4" s="19">
-        <f>Q4</f>
-        <v>2.5000000000000001E-2</v>
+        <f>P4</f>
+        <v>2.3E-2</v>
       </c>
       <c r="P4" s="79">
         <v>2.3E-2</v>
@@ -1749,12 +1980,12 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="S4" s="44">
-        <f>1-(1+O4)/(1+N4)</f>
-        <v>-7.1055381400208839E-2</v>
+        <f>M4-(AVERAGE(P4,R4))</f>
+        <v>-5.0999999999999997E-2</v>
       </c>
       <c r="T4" s="80">
         <f>S4*L4</f>
-        <v>-3.552769070010442E-2</v>
+        <v>-2.5499999999999998E-2</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
@@ -1765,6 +1996,7 @@
       <c r="F5" s="23"/>
       <c r="G5" s="41"/>
       <c r="H5" s="30"/>
+      <c r="S5" s="2"/>
     </row>
     <row r="6" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
@@ -1774,70 +2006,71 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="L6" s="121" t="s">
+      <c r="L6" s="112" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="121"/>
-      <c r="N6" s="121"/>
-      <c r="O6" s="121"/>
-      <c r="P6" s="121"/>
-      <c r="Q6" s="121"/>
+      <c r="M6" s="112"/>
+      <c r="N6" s="112"/>
+      <c r="O6" s="112"/>
+      <c r="P6" s="112"/>
+      <c r="Q6" s="112"/>
+      <c r="S6" s="2"/>
     </row>
     <row r="7" spans="2:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="114" t="s">
+      <c r="B7" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="112" t="s">
+      <c r="C7" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="112" t="s">
+      <c r="D7" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="112" t="s">
+      <c r="E7" s="113" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="112" t="s">
+      <c r="F7" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="112" t="s">
+      <c r="G7" s="113" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="112" t="s">
+      <c r="H7" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="112" t="s">
+      <c r="I7" s="113" t="s">
         <v>80</v>
       </c>
-      <c r="J7" s="112" t="s">
+      <c r="J7" s="113" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="112" t="s">
+      <c r="K7" s="113" t="s">
         <v>14</v>
       </c>
       <c r="L7" s="105" t="s">
         <v>105</v>
       </c>
-      <c r="M7" s="118" t="s">
+      <c r="M7" s="121" t="s">
         <v>83</v>
       </c>
-      <c r="N7" s="119"/>
-      <c r="O7" s="120"/>
-      <c r="P7" s="116" t="s">
+      <c r="N7" s="122"/>
+      <c r="O7" s="123"/>
+      <c r="P7" s="119" t="s">
         <v>82</v>
       </c>
-      <c r="Q7" s="117"/>
+      <c r="Q7" s="120"/>
     </row>
     <row r="8" spans="2:20" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="115"/>
-      <c r="C8" s="113"/>
-      <c r="D8" s="113"/>
-      <c r="E8" s="113"/>
-      <c r="F8" s="113"/>
-      <c r="G8" s="113"/>
-      <c r="H8" s="113"/>
-      <c r="I8" s="113"/>
-      <c r="J8" s="113"/>
-      <c r="K8" s="113"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="114"/>
+      <c r="E8" s="114"/>
+      <c r="F8" s="114"/>
+      <c r="G8" s="114"/>
+      <c r="H8" s="114"/>
+      <c r="I8" s="114"/>
+      <c r="J8" s="114"/>
+      <c r="K8" s="114"/>
       <c r="L8" s="106">
         <v>60000</v>
       </c>
@@ -2425,15 +2658,15 @@
       <c r="L20" s="105" t="s">
         <v>105</v>
       </c>
-      <c r="M20" s="118" t="s">
+      <c r="M20" s="121" t="s">
         <v>83</v>
       </c>
-      <c r="N20" s="119"/>
-      <c r="O20" s="120"/>
-      <c r="P20" s="110" t="s">
+      <c r="N20" s="122"/>
+      <c r="O20" s="123"/>
+      <c r="P20" s="115" t="s">
         <v>82</v>
       </c>
-      <c r="Q20" s="111"/>
+      <c r="Q20" s="116"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D21" s="2"/>
@@ -2732,27 +2965,27 @@
       </c>
       <c r="L32" s="101">
         <f>L31+$S$4</f>
-        <v>-7.4518827962664055E-2</v>
+        <v>-5.4463446562455206E-2</v>
       </c>
       <c r="M32" s="101">
         <f>M31+$S$4</f>
-        <v>-8.2600203275059542E-2</v>
+        <v>-6.2544821874850706E-2</v>
       </c>
       <c r="N32" s="102">
         <f>N31+$S$4</f>
-        <v>-9.0681578587455042E-2</v>
+        <v>-7.0626197187246192E-2</v>
       </c>
       <c r="O32" s="102">
         <f>O31+$S$4</f>
-        <v>-9.8762953899850542E-2</v>
+        <v>-7.8707572499641693E-2</v>
       </c>
       <c r="P32" s="101">
         <f>P31+$T$4</f>
-        <v>-0.13365867663633541</v>
+        <v>-0.12363098593623099</v>
       </c>
       <c r="Q32" s="103">
         <f>Q31+$T$4</f>
-        <v>-0.16252073132346218</v>
+        <v>-0.15249304062335775</v>
       </c>
     </row>
     <row r="33" spans="11:17" x14ac:dyDescent="0.25">
@@ -2764,6 +2997,7 @@
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="M35" s="126"/>
       <c r="Q35" s="5"/>
     </row>
     <row r="37" spans="11:17" x14ac:dyDescent="0.25">
@@ -2822,6 +3056,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M20:O20"/>
     <mergeCell ref="L6:Q6"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="G7:G8"/>
@@ -2830,13 +3071,6 @@
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M20:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2844,14 +3078,986 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD8DC36-9FEB-41D5-8A4B-4604E7733A2F}">
+  <dimension ref="B2:R47"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="12" width="26.7109375" customWidth="1"/>
+    <col min="13" max="17" width="19.7109375" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="105" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="111" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="111" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="L3" s="111" t="s">
+        <v>104</v>
+      </c>
+      <c r="M3" s="111" t="s">
+        <v>102</v>
+      </c>
+      <c r="N3" s="110" t="s">
+        <v>98</v>
+      </c>
+      <c r="O3" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="P3" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q3" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="R3" s="76" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="141">
+        <f>21000*1000000000</f>
+        <v>21000000000000</v>
+      </c>
+      <c r="C4" s="17">
+        <v>10487101.84</v>
+      </c>
+      <c r="D4" s="18">
+        <f>C4/80</f>
+        <v>131088.77299999999</v>
+      </c>
+      <c r="E4" s="17">
+        <v>9763</v>
+      </c>
+      <c r="F4" s="17">
+        <v>20292</v>
+      </c>
+      <c r="G4" s="72">
+        <v>2.3E-2</v>
+      </c>
+      <c r="H4" s="44">
+        <f>0.05-G4</f>
+        <v>2.7000000000000003E-2</v>
+      </c>
+      <c r="I4" s="45">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J4" s="46">
+        <v>0.19</v>
+      </c>
+      <c r="K4" s="148">
+        <v>686158</v>
+      </c>
+      <c r="L4" s="19">
+        <v>-3.7999999999999999E-2</v>
+      </c>
+      <c r="M4" s="19">
+        <v>-4.2999999999999997E-2</v>
+      </c>
+      <c r="N4" s="79">
+        <f>O4</f>
+        <v>2.3E-2</v>
+      </c>
+      <c r="O4" s="19">
+        <v>2.3E-2</v>
+      </c>
+      <c r="P4" s="19">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="Q4" s="140">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="R4" s="77">
+        <f>1-(1+N4)/(1+M4)</f>
+        <v>-6.8965517241379226E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="30"/>
+    </row>
+    <row r="6" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="L6" s="109"/>
+    </row>
+    <row r="7" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="117" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="113" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="113" t="s">
+        <v>122</v>
+      </c>
+      <c r="G7" s="113" t="s">
+        <v>118</v>
+      </c>
+      <c r="H7" s="113" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="121" t="s">
+        <v>123</v>
+      </c>
+      <c r="K7" s="122"/>
+      <c r="L7" s="120"/>
+    </row>
+    <row r="8" spans="2:18" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="118"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="114"/>
+      <c r="E8" s="114"/>
+      <c r="F8" s="114"/>
+      <c r="G8" s="114"/>
+      <c r="H8" s="114"/>
+      <c r="I8" s="114"/>
+      <c r="J8" s="105" t="s">
+        <v>119</v>
+      </c>
+      <c r="K8" s="105" t="s">
+        <v>121</v>
+      </c>
+      <c r="L8" s="105" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="24">
+        <v>6604958</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="24">
+        <v>103468</v>
+      </c>
+      <c r="F9" s="25">
+        <f>E9/SUM($E$9:$E$19)</f>
+        <v>0.31050491409708153</v>
+      </c>
+      <c r="G9" s="24">
+        <f>(E9/C9)*100000</f>
+        <v>1566.5201807490675</v>
+      </c>
+      <c r="H9" s="28">
+        <v>4.8976565193009201</v>
+      </c>
+      <c r="I9" s="29">
+        <f>H9*$D$4</f>
+        <v>642027.78369060834</v>
+      </c>
+      <c r="J9" s="107">
+        <f>E9*I9</f>
+        <v>66429330722.899864</v>
+      </c>
+      <c r="K9" s="107">
+        <f>$F9*K$24*$I9</f>
+        <v>68923632729.066635</v>
+      </c>
+      <c r="L9" s="107">
+        <f>$F9*L$24*$I9</f>
+        <v>79380284194.017532</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="24">
+        <v>15969872</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="24">
+        <v>87369</v>
+      </c>
+      <c r="F10" s="25">
+        <f>E10/SUM($E$9:$E$19)</f>
+        <v>0.26219221246905244</v>
+      </c>
+      <c r="G10" s="24">
+        <f>(E10/C10)*100000</f>
+        <v>547.08641371702913</v>
+      </c>
+      <c r="H10" s="28">
+        <v>9.6420808894931902</v>
+      </c>
+      <c r="I10" s="29">
+        <f>H10*$D$4</f>
+        <v>1263968.5529704108</v>
+      </c>
+      <c r="J10" s="107">
+        <f>E10*I10</f>
+        <v>110431668504.47182</v>
+      </c>
+      <c r="K10" s="107">
+        <f>$F10*K$24*$I10</f>
+        <v>114578179229.44128</v>
+      </c>
+      <c r="L10" s="107">
+        <f>$F10*L$24*$I10</f>
+        <v>131961245650.22324</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="24">
+        <v>31483433</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="24">
+        <v>71779</v>
+      </c>
+      <c r="F11" s="25">
+        <f>E11/SUM($E$9:$E$19)</f>
+        <v>0.21540700727736514</v>
+      </c>
+      <c r="G11" s="24">
+        <f>(E11/C11)*100000</f>
+        <v>227.98974940248735</v>
+      </c>
+      <c r="H11" s="28">
+        <v>16.0394166284938</v>
+      </c>
+      <c r="I11" s="29">
+        <f>H11*$D$4</f>
+        <v>2102587.4454650488</v>
+      </c>
+      <c r="J11" s="107">
+        <f>E11*I11</f>
+        <v>150921624248.03574</v>
+      </c>
+      <c r="K11" s="107">
+        <f>$F11*K$24*$I11</f>
+        <v>156588460057.44806</v>
+      </c>
+      <c r="L11" s="107">
+        <f>$F11*L$24*$I11</f>
+        <v>180345056821.44302</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="24">
+        <v>42448537</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="24">
+        <v>42320</v>
+      </c>
+      <c r="F12" s="25">
+        <f>E12/SUM($E$9:$E$19)</f>
+        <v>0.12700127541450973</v>
+      </c>
+      <c r="G12" s="24">
+        <f>(E12/C12)*100000</f>
+        <v>99.697193333188366</v>
+      </c>
+      <c r="H12" s="28">
+        <v>23.605006871114799</v>
+      </c>
+      <c r="I12" s="29">
+        <f>H12*$D$4</f>
+        <v>3094351.387391008</v>
+      </c>
+      <c r="J12" s="107">
+        <f>E12*I12</f>
+        <v>130952950714.38745</v>
+      </c>
+      <c r="K12" s="107">
+        <f>$F12*K$24*$I12</f>
+        <v>135869998713.00227</v>
+      </c>
+      <c r="L12" s="107">
+        <f>$F12*L$24*$I12</f>
+        <v>156483323414.9957</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="24">
+        <v>40874902</v>
+      </c>
+      <c r="D13" s="25"/>
+      <c r="E13" s="24">
+        <v>17946</v>
+      </c>
+      <c r="F13" s="25">
+        <f>E13/SUM($E$9:$E$19)</f>
+        <v>5.3855503038487511E-2</v>
+      </c>
+      <c r="G13" s="24">
+        <f>(E13/C13)*100000</f>
+        <v>43.904692419813017</v>
+      </c>
+      <c r="H13" s="28">
+        <v>31.981264625350299</v>
+      </c>
+      <c r="I13" s="29">
+        <f>H13*$D$4</f>
+        <v>4192384.738725475</v>
+      </c>
+      <c r="J13" s="107">
+        <f>E13*I13</f>
+        <v>75236536521.167374</v>
+      </c>
+      <c r="K13" s="107">
+        <f>$F13*K$24*$I13</f>
+        <v>78061533279.972534</v>
+      </c>
+      <c r="L13" s="107">
+        <f>$F13*L$24*$I13</f>
+        <v>89904528403.822159</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="24">
+        <v>41659144</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="24">
+        <v>6891</v>
+      </c>
+      <c r="F14" s="25">
+        <f>E14/SUM($E$9:$E$19)</f>
+        <v>2.0679720909295519E-2</v>
+      </c>
+      <c r="G14" s="24">
+        <f>(E14/C14)*100000</f>
+        <v>16.541386448074881</v>
+      </c>
+      <c r="H14" s="28">
+        <v>41.020805174987501</v>
+      </c>
+      <c r="I14" s="29">
+        <f>H14*$D$4</f>
+        <v>5377367.0178611614</v>
+      </c>
+      <c r="J14" s="107">
+        <f>E14*I14</f>
+        <v>37055436120.081261</v>
+      </c>
+      <c r="K14" s="107">
+        <f>$F14*K$24*$I14</f>
+        <v>38446801163.923882</v>
+      </c>
+      <c r="L14" s="107">
+        <f>$F14*L$24*$I14</f>
+        <v>44279703229.515068</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="24">
+        <v>45940321</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="E15" s="24">
+        <v>2707</v>
+      </c>
+      <c r="F15" s="25">
+        <f>E15/SUM($E$9:$E$19)</f>
+        <v>8.1236401830594943E-3</v>
+      </c>
+      <c r="G15" s="24">
+        <f>(E15/C15)*100000</f>
+        <v>5.8924272644938638</v>
+      </c>
+      <c r="H15" s="28">
+        <v>50.307388524170001</v>
+      </c>
+      <c r="I15" s="29">
+        <f>H15*$D$4</f>
+        <v>6594733.8344677258</v>
+      </c>
+      <c r="J15" s="107">
+        <f>E15*I15</f>
+        <v>17851944489.904133</v>
+      </c>
+      <c r="K15" s="107">
+        <f>$F15*K$24*$I15</f>
+        <v>18522252928.519726</v>
+      </c>
+      <c r="L15" s="107">
+        <f>$F15*L$24*$I15</f>
+        <v>21332330336.664196</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="24">
+        <v>42687510</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="24">
+        <v>611</v>
+      </c>
+      <c r="F16" s="25">
+        <f>E16/SUM($E$9:$E$19)</f>
+        <v>1.833595918673569E-3</v>
+      </c>
+      <c r="G16" s="24">
+        <f>(E16/C16)*100000</f>
+        <v>1.4313320219427181</v>
+      </c>
+      <c r="H16" s="28">
+        <v>59.748654295544497</v>
+      </c>
+      <c r="I16" s="29">
+        <f>H16*$D$4</f>
+        <v>7832377.7800041065</v>
+      </c>
+      <c r="J16" s="107">
+        <f>E16*I16</f>
+        <v>4785582823.582509</v>
+      </c>
+      <c r="K16" s="107">
+        <f>$F16*K$24*$I16</f>
+        <v>4965272859.7102432</v>
+      </c>
+      <c r="L16" s="107">
+        <f>$F16*L$24*$I16</f>
+        <v>5718572209.5350571</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="24">
+        <v>40994163</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="24">
+        <v>66</v>
+      </c>
+      <c r="F17" s="25">
+        <f>E17/SUM($E$9:$E$19)</f>
+        <v>1.9806437092054918E-4</v>
+      </c>
+      <c r="G17" s="24">
+        <f>(E17/C17)*100000</f>
+        <v>0.16099853044932275</v>
+      </c>
+      <c r="H17" s="28">
+        <v>69.534184762763402</v>
+      </c>
+      <c r="I17" s="29">
+        <f>H17*$D$4</f>
+        <v>9115150.9621059503</v>
+      </c>
+      <c r="J17" s="107">
+        <f>E17*I17</f>
+        <v>601599963.49899268</v>
+      </c>
+      <c r="K17" s="107">
+        <f>$F17*K$24*$I17</f>
+        <v>624188961.1531285</v>
+      </c>
+      <c r="L17" s="107">
+        <f>$F17*L$24*$I17</f>
+        <v>718886906.6416502</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="125" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="24">
+        <v>15793631</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="24">
+        <v>24</v>
+      </c>
+      <c r="F18" s="25">
+        <f>E18/SUM($E$9:$E$19)</f>
+        <v>7.2023407607472431E-5</v>
+      </c>
+      <c r="G18" s="24">
+        <f>(E18/C18)*100000</f>
+        <v>0.15195998944131339</v>
+      </c>
+      <c r="H18" s="28">
+        <v>76.456815786792504</v>
+      </c>
+      <c r="I18" s="29">
+        <f>H18*$D$4</f>
+        <v>10022630.168977657</v>
+      </c>
+      <c r="J18" s="107">
+        <f>E18*I18</f>
+        <v>240543124.05546379</v>
+      </c>
+      <c r="K18" s="107">
+        <f>$F18*K$24*$I18</f>
+        <v>249575086.14768964</v>
+      </c>
+      <c r="L18" s="107">
+        <f>$F18*L$24*$I18</f>
+        <v>287439017.38358504</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" s="34">
+        <v>3783052</v>
+      </c>
+      <c r="D19" s="35"/>
+      <c r="E19" s="34">
+        <v>44</v>
+      </c>
+      <c r="F19" s="35">
+        <f>E19/SUM($E$9:$E$19)</f>
+        <v>1.3204291394703279E-4</v>
+      </c>
+      <c r="G19" s="34">
+        <f>(E19/C19)*100000</f>
+        <v>1.1630820829319819</v>
+      </c>
+      <c r="H19" s="38">
+        <v>78.465000000000003</v>
+      </c>
+      <c r="I19" s="18">
+        <f>H19*$D$4</f>
+        <v>10285880.573445</v>
+      </c>
+      <c r="J19" s="108">
+        <f>E19*I19</f>
+        <v>452578745.23158002</v>
+      </c>
+      <c r="K19" s="108">
+        <f>$F19*K$24*$I19</f>
+        <v>469572263.90616184</v>
+      </c>
+      <c r="L19" s="108">
+        <f>$F19*L$24*$I19</f>
+        <v>540812755.83693552</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="124"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="124"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
+    </row>
+    <row r="22" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="40"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="81" t="s">
+        <v>97</v>
+      </c>
+      <c r="J22" s="109"/>
+    </row>
+    <row r="23" spans="2:17" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="105" t="s">
+        <v>119</v>
+      </c>
+      <c r="K23" s="105" t="s">
+        <v>121</v>
+      </c>
+      <c r="L23" s="105" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="D24" s="2"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="82" t="s">
+        <v>89</v>
+      </c>
+      <c r="J24" s="127">
+        <f>SUM(E9:E19)</f>
+        <v>333225</v>
+      </c>
+      <c r="K24" s="127">
+        <v>345737</v>
+      </c>
+      <c r="L24" s="127">
+        <v>398190</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="J25" s="128">
+        <f>J24*($H$4/$G$4)</f>
+        <v>391177.17391304352</v>
+      </c>
+      <c r="K25" s="128">
+        <f>K24*($H$4/$G$4)</f>
+        <v>405865.17391304352</v>
+      </c>
+      <c r="L25" s="128">
+        <f>L24*($H$4/$G$4)</f>
+        <v>467440.43478260876</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="H26" s="4"/>
+      <c r="I26" s="94" t="s">
+        <v>91</v>
+      </c>
+      <c r="J26" s="129">
+        <f>SUM(J24,J25)*($I$4/($G$4+$H$4))</f>
+        <v>2028326.086956522</v>
+      </c>
+      <c r="K26" s="129">
+        <f>SUM(K24,K25)*($I$4/($G$4+$H$4))</f>
+        <v>2104486.086956522</v>
+      </c>
+      <c r="L26" s="129">
+        <f>SUM(L24,L25)*($I$4/($G$4+$H$4))</f>
+        <v>2423765.2173913047</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H27" s="4"/>
+      <c r="I27" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="J27" s="130">
+        <f>SUM(J8,J24,J26)</f>
+        <v>2361551.086956522</v>
+      </c>
+      <c r="K27" s="130">
+        <f>SUM(J8,K24,K26)</f>
+        <v>2450223.086956522</v>
+      </c>
+      <c r="L27" s="130">
+        <f>SUM(K8,L24,L26)</f>
+        <v>2821955.2173913047</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H28" s="4"/>
+      <c r="I28" s="131"/>
+      <c r="J28" s="132"/>
+      <c r="K28" s="132"/>
+      <c r="L28" s="132"/>
+    </row>
+    <row r="29" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H29" s="4"/>
+      <c r="I29" s="133" t="s">
+        <v>79</v>
+      </c>
+      <c r="J29" s="64"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="64"/>
+    </row>
+    <row r="30" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="I30" s="142" t="s">
+        <v>69</v>
+      </c>
+      <c r="J30" s="134">
+        <f>SUM(J9:J19)</f>
+        <v>594959795977.31616</v>
+      </c>
+      <c r="K30" s="134">
+        <f>SUM(K9:K19)</f>
+        <v>617299467272.2915</v>
+      </c>
+      <c r="L30" s="134">
+        <f>SUM(L9:L19)</f>
+        <v>710952182940.078</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="I31" s="143" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="135">
+        <f>J26*$E$4</f>
+        <v>19802547586.956524</v>
+      </c>
+      <c r="K31" s="135">
+        <f>K26*$E$4</f>
+        <v>20546097666.956524</v>
+      </c>
+      <c r="L31" s="135">
+        <f>L26*$E$4</f>
+        <v>23663219817.391308</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="I32" s="144" t="s">
+        <v>51</v>
+      </c>
+      <c r="J32" s="136">
+        <f>SUM(J24,J25)*$F$4</f>
+        <v>14699568913.043478</v>
+      </c>
+      <c r="K32" s="136">
+        <f>SUM(K24,K25)*$F$4</f>
+        <v>15251511313.043478</v>
+      </c>
+      <c r="L32" s="136">
+        <f>SUM(L24,L25)*$F$4</f>
+        <v>17565372782.608696</v>
+      </c>
+    </row>
+    <row r="33" spans="9:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="I33" s="145" t="s">
+        <v>85</v>
+      </c>
+      <c r="J33" s="137">
+        <f t="shared" ref="J33" si="0">SUM(J30:J32)</f>
+        <v>629461912477.31616</v>
+      </c>
+      <c r="K33" s="137">
+        <f t="shared" ref="K33:L33" si="1">SUM(K30:K32)</f>
+        <v>653097076252.2915</v>
+      </c>
+      <c r="L33" s="137">
+        <f t="shared" si="1"/>
+        <v>752180775540.078</v>
+      </c>
+    </row>
+    <row r="34" spans="9:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I34" s="146" t="s">
+        <v>70</v>
+      </c>
+      <c r="J34" s="138">
+        <f>J33/$B$4*-1</f>
+        <v>-2.9974376784634101E-2</v>
+      </c>
+      <c r="K34" s="138">
+        <f>K33/$B$4*-1</f>
+        <v>-3.1099860773918644E-2</v>
+      </c>
+      <c r="L34" s="138">
+        <f>L33/$B$4*-1</f>
+        <v>-3.5818132168575142E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="9:17" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I35" s="147" t="s">
+        <v>86</v>
+      </c>
+      <c r="J35" s="139">
+        <f>J34+$R$4</f>
+        <v>-9.8939894026013331E-2</v>
+      </c>
+      <c r="K35" s="139">
+        <f>K34+$R$4</f>
+        <v>-0.10006537801529787</v>
+      </c>
+      <c r="L35" s="139">
+        <f>L34+$R$4</f>
+        <v>-0.10478364940995437</v>
+      </c>
+    </row>
+    <row r="36" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="P37" s="2"/>
+    </row>
+    <row r="38" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="Q38" s="5"/>
+    </row>
+    <row r="40" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="K40" s="2"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="6"/>
+    </row>
+    <row r="41" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="K41" s="3"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+    </row>
+    <row r="42" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+    </row>
+    <row r="44" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+    </row>
+    <row r="45" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+    </row>
+    <row r="46" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+    </row>
+    <row r="47" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="H7:H8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7BF6D1-AC08-47EC-B644-0F220400F590}">
-  <dimension ref="A2:C26"/>
+  <dimension ref="A2:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3129,6 +4335,17 @@
       </c>
       <c r="C26" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3161,7 +4378,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BC6753-CC5F-45A2-9E6F-A8F26D094679}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>